<commit_message>
UPDATE IN EXCEL READER,CONFIG FILE,CONFIG PROP
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Team_08_API Architects_LMSTestData.xlsx
+++ b/src/test/resources/TestData/Team_08_API Architects_LMSTestData.xlsx
@@ -1,13 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\priya\git\Team_08_APIArchitects_RestAssured\src\test\resources\TestData\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D35513BF-F653-4832-8CF2-7DD742D425A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Login" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="PythonArray" sheetId="2" r:id="rId5"/>
+    <sheet name="Login" sheetId="1" r:id="rId1"/>
+    <sheet name="Program" sheetId="3" r:id="rId2"/>
+    <sheet name="Batch" sheetId="4" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="5" r:id="rId4"/>
+    <sheet name="PythonArray" sheetId="2" r:id="rId5"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataChecksum="xiQ+14SZppxkpB3hF2CpN5YgPYHGoCsLamLy7CqNZLI="/>
@@ -17,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Username</t>
   </si>
@@ -66,26 +78,61 @@
   <si>
     <t>search(input_list,num)</t>
   </si>
+  <si>
+    <t>programDescription</t>
+  </si>
+  <si>
+    <t>programName</t>
+  </si>
+  <si>
+    <t>programStatus</t>
+  </si>
+  <si>
+    <t>Selenium Classes</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>programId</t>
+  </si>
+  <si>
+    <t>ABCD1</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Menlo"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -93,7 +140,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -103,37 +150,42 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+  <cellXfs count="5">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -323,60 +375,136 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <cols>
+    <col min="1" max="1" width="30.5703125" customWidth="1"/>
+    <col min="2" max="2" width="27.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{287BA625-3A1E-4F32-910C-057B33D91932}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="22" customWidth="1"/>
+    <col min="2" max="2" width="25.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6792F2D-317A-4B56-B3C6-819C430D682E}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0973ABCC-0DFB-4CD7-A279-D6A93CDE91D4}">
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
-  <cols>
-    <col customWidth="1" min="1" max="1" width="30.57"/>
-    <col customWidth="1" min="2" max="2" width="27.86"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-  </sheetData>
-  <drawing r:id="rId1"/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="48.43"/>
-    <col customWidth="1" min="2" max="2" width="33.71"/>
-    <col customWidth="1" min="3" max="26" width="8.71"/>
+    <col min="1" max="1" width="48.42578125" customWidth="1"/>
+    <col min="2" max="2" width="33.7109375" customWidth="1"/>
+    <col min="3" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -384,7 +512,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -392,50 +520,48 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:2">
       <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:2">
       <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
     </row>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Coded For User Module  - For creating User Id with Role- Tricky one. Done. Admin user id  is generating.
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Team_08_API Architects_LMSTestData.xlsx
+++ b/src/test/resources/TestData/Team_08_API Architects_LMSTestData.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="Login" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="PythonArray" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="UserModule" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="41">
   <si>
     <t>Username</t>
   </si>
@@ -25,53 +25,128 @@
     <t>Password</t>
   </si>
   <si>
+    <t>InvalidUsername</t>
+  </si>
+  <si>
+    <t>InvalidPassword</t>
+  </si>
+  <si>
     <t>numpyninja@gmail.com</t>
   </si>
   <si>
     <t>lmsHackathon@2024</t>
   </si>
   <si>
-    <t>PythonCode for Array in tryedior arrays in python</t>
-  </si>
-  <si>
-    <t>Expected Output</t>
-  </si>
-  <si>
-    <t>def search(input_list, num):</t>
-  </si>
-  <si>
-    <t>564 is Number is Not Found</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  output = 'Number is Not Found'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  for x in input_list:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    if x == num:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      output = 'Number is found'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    print(str(num) + ' is '+output)</t>
-  </si>
-  <si>
-    <t>input_list=[12,23,45,56,67]</t>
-  </si>
-  <si>
-    <t>num=564</t>
-  </si>
-  <si>
-    <t>search(input_list,num)</t>
+    <t>abc</t>
+  </si>
+  <si>
+    <t>UserComments</t>
+  </si>
+  <si>
+    <t>UserEduPg</t>
+  </si>
+  <si>
+    <t>UserEduUg</t>
+  </si>
+  <si>
+    <t>UserFirstName</t>
+  </si>
+  <si>
+    <t>UserId</t>
+  </si>
+  <si>
+    <t>UserLastName</t>
+  </si>
+  <si>
+    <t>UserLinkedinUrl</t>
+  </si>
+  <si>
+    <t>UserLocation</t>
+  </si>
+  <si>
+    <t>UserLogin</t>
+  </si>
+  <si>
+    <t>LoginStatus</t>
+  </si>
+  <si>
+    <t>RoleIds</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>UserLoginEmail</t>
+  </si>
+  <si>
+    <t>UserMiddleName</t>
+  </si>
+  <si>
+    <t>UserPhoneNumber</t>
+  </si>
+  <si>
+    <t>UserRoleMaps</t>
+  </si>
+  <si>
+    <t>RoleId</t>
+  </si>
+  <si>
+    <t>UserRoleStatus</t>
+  </si>
+  <si>
+    <t>UserTimeZone</t>
+  </si>
+  <si>
+    <t>UserVisaStatus</t>
+  </si>
+  <si>
+    <t>CreatingAdminRole</t>
+  </si>
+  <si>
+    <t>EEE</t>
+  </si>
+  <si>
+    <t>Computer Science</t>
+  </si>
+  <si>
+    <t>TeamAPIARCHITECT</t>
+  </si>
+  <si>
+    <t>Team</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/EndpointExplorer_007/</t>
+  </si>
+  <si>
+    <t>Georgia</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>Testuser</t>
+  </si>
+  <si>
+    <t>abcgfhjefergge</t>
+  </si>
+  <si>
+    <t>API</t>
+  </si>
+  <si>
+    <t>R01</t>
+  </si>
+  <si>
+    <t>EST</t>
+  </si>
+  <si>
+    <t>H1B</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+  <fonts count="10">
     <font>
       <sz val="11.0"/>
       <color rgb="FF000000"/>
@@ -83,12 +158,48 @@
       <name val="Calibri"/>
     </font>
     <font>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="12.0"/>
       <color rgb="FF000000"/>
       <name val="Menlo"/>
     </font>
+    <font>
+      <sz val="9.0"/>
+      <color rgb="FF9CDCFE"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="8.0"/>
+      <color rgb="FF000000"/>
+      <name val="&quot;Helvetica Neue&quot;"/>
+    </font>
+    <font>
+      <sz val="9.0"/>
+      <color rgb="FFCE9178"/>
+      <name val="IBMPlexMono"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="9.0"/>
+      <color rgb="FFCE9178"/>
+      <name val="IBMPlexMono"/>
+    </font>
+    <font>
+      <sz val="9.0"/>
+      <color rgb="FFCE9178"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="9.0"/>
+      <color rgb="FFB5CEA8"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -101,6 +212,12 @@
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF212121"/>
+        <bgColor rgb="FF212121"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border/>
@@ -108,12 +225,34 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="11">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
+    <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -347,13 +486,25 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>3</v>
+      <c r="A2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -377,65 +528,154 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>5</v>
+      <c r="A1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="R1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="S1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="T1" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="U1" s="5" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>7</v>
+      <c r="A2" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="M2" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="N2" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="P2" s="10">
+        <v>4.56768855E8</v>
+      </c>
+      <c r="R2" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="S2" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="T2" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="U2" s="7" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="A3" s="1"/>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="s">
-        <v>9</v>
-      </c>
+      <c r="A4" s="1"/>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="A5" s="1"/>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="s">
-        <v>11</v>
-      </c>
+      <c r="A6" s="1"/>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="A7" s="1"/>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="s">
-        <v>13</v>
-      </c>
+      <c r="A8" s="1"/>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="A9" s="1"/>
     </row>
     <row r="10">
-      <c r="A10" s="1" t="s">
-        <v>15</v>
-      </c>
+      <c r="A10" s="1"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink r:id="rId1" ref="G2"/>
+  </hyperlinks>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
ignore batch validation and try to copy rest
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Team_08_API Architects_LMSTestData.xlsx
+++ b/src/test/resources/TestData/Team_08_API Architects_LMSTestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\priya\git\Team_08_APIArchitects_RestAssured\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D35513BF-F653-4832-8CF2-7DD742D425A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22CD3186-61C2-42D8-AFE5-66F117055ECC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
   <si>
     <t>Username</t>
   </si>
@@ -82,9 +82,6 @@
     <t>programDescription</t>
   </si>
   <si>
-    <t>programName</t>
-  </si>
-  <si>
     <t>programStatus</t>
   </si>
   <si>
@@ -97,7 +94,13 @@
     <t>programId</t>
   </si>
   <si>
-    <t>ABCD1</t>
+    <t>BatchDescription</t>
+  </si>
+  <si>
+    <t>BatchNoOfClasses</t>
+  </si>
+  <si>
+    <t>BatchStatus</t>
   </si>
 </sst>
 </file>
@@ -420,61 +423,84 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{287BA625-3A1E-4F32-910C-057B33D91932}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1"/>
-    <col min="2" max="2" width="25.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6792F2D-317A-4B56-B3C6-819C430D682E}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="17.42578125" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="3" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="3"/>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
         <v>18</v>
       </c>
-      <c r="D1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="4" t="s">
+      <c r="B2">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6792F2D-317A-4B56-B3C6-819C430D682E}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
ignore batch validation for now
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Team_08_API Architects_LMSTestData.xlsx
+++ b/src/test/resources/TestData/Team_08_API Architects_LMSTestData.xlsx
@@ -3,12 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\priya\git\Team_08_APIArchitects_RestAssured\src\test\resources\TestData\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22CD3186-61C2-42D8-AFE5-66F117055ECC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{AD128BFD-FE12-468B-A415-495FB9E253D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,6 +15,7 @@
     <sheet name="PythonArray" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataChecksum="xiQ+14SZppxkpB3hF2CpN5YgPYHGoCsLamLy7CqNZLI="/>
@@ -29,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
   <si>
     <t>Username</t>
   </si>
@@ -101,6 +97,18 @@
   </si>
   <si>
     <t>BatchStatus</t>
+  </si>
+  <si>
+    <t>BatchNoOfClassesmissingadditonalfield</t>
+  </si>
+  <si>
+    <t>BatchStatusmissingadditonalfield</t>
+  </si>
+  <si>
+    <t>BatchDescriptionmissingadditionalfield</t>
+  </si>
+  <si>
+    <t>null</t>
   </si>
 </sst>
 </file>
@@ -463,10 +471,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6792F2D-317A-4B56-B3C6-819C430D682E}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -474,10 +482,12 @@
     <col min="1" max="1" width="17.42578125" customWidth="1"/>
     <col min="2" max="2" width="18.85546875" customWidth="1"/>
     <col min="3" max="3" width="14.7109375" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" customWidth="1"/>
+    <col min="4" max="4" width="38.5703125" customWidth="1"/>
+    <col min="5" max="5" width="30.7109375" customWidth="1"/>
+    <col min="6" max="6" width="35.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:7">
       <c r="A1" s="3" t="s">
         <v>21</v>
       </c>
@@ -487,9 +497,18 @@
       <c r="C1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="3"/>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="D1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" s="4"/>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -498,6 +517,15 @@
       </c>
       <c r="C2" t="s">
         <v>19</v>
+      </c>
+      <c r="D2">
+        <v>4</v>
+      </c>
+      <c r="E2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Schema validation,Status code Validation, HeaderValidation. Added everything as common validation . can be used across all modules.
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Team_08_API Architects_LMSTestData.xlsx
+++ b/src/test/resources/TestData/Team_08_API Architects_LMSTestData.xlsx
@@ -28,10 +28,52 @@
     <t>Excel Worksheet Name</t>
   </si>
   <si>
+    <t>Export Summary</t>
+  </si>
+  <si>
+    <t>Table 1</t>
+  </si>
+  <si>
     <t>Login</t>
   </si>
   <si>
-    <t>Table 1</t>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="12"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>Login</t>
+    </r>
+  </si>
+  <si>
+    <t>UserModule</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="12"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>UserModule</t>
+    </r>
+  </si>
+  <si>
+    <t>UserModuleMandatory</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="12"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>UserModuleMandatory</t>
+    </r>
   </si>
   <si>
     <t>Username</t>
@@ -55,9 +97,6 @@
     <t>abc</t>
   </si>
   <si>
-    <t>UserModule</t>
-  </si>
-  <si>
     <t>UserComments</t>
   </si>
   <si>
@@ -82,9 +121,6 @@
     <t>UserLocation</t>
   </si>
   <si>
-    <t>UserLogin</t>
-  </si>
-  <si>
     <t>LoginStatus</t>
   </si>
   <si>
@@ -94,16 +130,7 @@
     <t>Status</t>
   </si>
   <si>
-    <t>UserLoginEmail</t>
-  </si>
-  <si>
     <t>UserMiddleName</t>
-  </si>
-  <si>
-    <t>UserPhoneNumber</t>
-  </si>
-  <si>
-    <t>UserRoleMaps</t>
   </si>
   <si>
     <t>AdminRoleId</t>
@@ -153,22 +180,19 @@
     <t>Testuser</t>
   </si>
   <si>
-    <t>abcgfhjefergge</t>
+    <t>R01</t>
   </si>
   <si>
     <t>API</t>
   </si>
   <si>
-    <t>R01</t>
-  </si>
-  <si>
     <t>EST</t>
   </si>
   <si>
     <t>H1B</t>
   </si>
   <si>
-    <t>UserModuleMandatory</t>
+    <t>UserLogin</t>
   </si>
   <si>
     <t>CreatingWithMandatoryFields</t>
@@ -286,12 +310,99 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="14">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="12"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="12"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="12"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="12"/>
+      </right>
+      <top style="thin">
+        <color indexed="12"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="12"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="12"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="12"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="12"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="12"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="12"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="12"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -320,22 +431,6 @@
       <bottom style="thin">
         <color indexed="12"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="12"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -370,7 +465,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -392,59 +487,104 @@
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="6" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="6" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="4" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="4" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="4" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="4" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="4" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" readingOrder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="9" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="4" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="4" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="4" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="4" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -667,12 +807,12 @@
         <a:solidFill>
           <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -705,10 +845,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -956,12 +1096,12 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -1276,10 +1416,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1530,90 +1670,184 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="13" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="2" customWidth="1"/>
+    <col min="1" max="1" width="2" style="6" customWidth="1"/>
     <col min="2" max="4" width="30.5547" customWidth="1"/>
+    <col min="2" max="2" width="30.5" style="6" customWidth="1"/>
+    <col min="3" max="3" width="30.5" style="6" customWidth="1"/>
+    <col min="4" max="4" width="30.5" style="6" customWidth="1"/>
+    <col min="5" max="5" width="10" style="6" customWidth="1"/>
+    <col min="6" max="16384" width="10" style="6" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" ht="13.55" customHeight="1">
+      <c r="A1" s="7"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="9"/>
+    </row>
+    <row r="2" ht="13.55" customHeight="1">
+      <c r="A2" s="10"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="12"/>
+    </row>
     <row r="3" ht="50" customHeight="1">
-      <c r="B3" t="s" s="1">
+      <c r="A3" s="10"/>
+      <c r="B3" t="s" s="13">
         <v>0</v>
       </c>
-      <c r="C3"/>
-      <c r="D3"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="12"/>
+    </row>
+    <row r="4" ht="13.55" customHeight="1">
+      <c r="A4" s="10"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="12"/>
+    </row>
+    <row r="5" ht="13.55" customHeight="1">
+      <c r="A5" s="10"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="12"/>
+    </row>
+    <row r="6" ht="13.55" customHeight="1">
+      <c r="A6" s="10"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="12"/>
     </row>
     <row r="7">
-      <c r="B7" t="s" s="2">
+      <c r="A7" s="10"/>
+      <c r="B7" t="s" s="14">
         <v>1</v>
       </c>
-      <c r="C7" t="s" s="2">
+      <c r="C7" t="s" s="14">
         <v>2</v>
       </c>
-      <c r="D7" t="s" s="2">
+      <c r="D7" t="s" s="14">
         <v>3</v>
       </c>
+      <c r="E7" s="12"/>
+    </row>
+    <row r="8" ht="13.55" customHeight="1">
+      <c r="A8" s="10"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="12"/>
     </row>
     <row r="9">
-      <c r="B9" t="s" s="3">
-        <v>4</v>
-      </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
+      <c r="A9" s="10"/>
+      <c r="B9" t="s" s="15">
+        <v>6</v>
+      </c>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="12"/>
     </row>
     <row r="10">
-      <c r="B10" s="4"/>
-      <c r="C10" t="s" s="4">
+      <c r="A10" s="10"/>
+      <c r="B10" s="17"/>
+      <c r="C10" t="s" s="18">
         <v>5</v>
       </c>
-      <c r="D10" t="s" s="5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11">
+      <c r="D10" t="s" s="19">
+        <v>7</v>
+      </c>
+      <c r="E10" s="12"/>
+    </row>
+    <row r="11" ht="13" customHeight="1">
+      <c r="A11" s="10"/>
       <c r="B11" t="s" s="3">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
-    </row>
-    <row r="12">
+      <c r="E11" s="12"/>
+    </row>
+    <row r="12" ht="13" customHeight="1">
+      <c r="A12" s="10"/>
       <c r="B12" s="4"/>
       <c r="C12" t="s" s="4">
         <v>5</v>
       </c>
       <c r="D12" t="s" s="5">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13">
+        <v>6</v>
+      </c>
+      <c r="E12" s="12"/>
+    </row>
+    <row r="13" ht="13" customHeight="1">
+      <c r="A13" s="10"/>
       <c r="B13" t="s" s="3">
-        <v>48</v>
+        <v>8</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
-    </row>
-    <row r="14">
+      <c r="E13" s="12"/>
+    </row>
+    <row r="14" ht="13" customHeight="1">
+      <c r="A14" s="20"/>
       <c r="B14" s="4"/>
       <c r="C14" t="s" s="4">
         <v>5</v>
       </c>
       <c r="D14" t="s" s="5">
-        <v>48</v>
+        <v>8</v>
+      </c>
+      <c r="E14" s="24"/>
+    </row>
+    <row r="15">
+      <c r="B15" t="s" s="3">
+        <v>10</v>
+      </c>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+    </row>
+    <row r="16">
+      <c r="B16" s="4"/>
+      <c r="C16" t="s" s="4">
+        <v>5</v>
+      </c>
+      <c r="D16" t="s" s="5">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
+    <mergeCell ref="B3:D3"/>
     <mergeCell ref="B3:D3"/>
   </mergeCells>
   <hyperlinks>
+    <hyperlink ref="D10" location="'Export Summary'!R1C1" tooltip="" display="Export Summary"/>
     <hyperlink ref="D10" location="'Login'!R1C1" tooltip="" display="Login"/>
     <hyperlink ref="D12" location="'UserModule'!R1C1" tooltip="" display="UserModule"/>
     <hyperlink ref="D14" location="'UserModuleMandatory'!R1C1" tooltip="" display="UserModuleMandatory"/>
+    <hyperlink ref="D12" location="'Login'!R1C1" tooltip="" display="Login"/>
+    <hyperlink ref="D14" location="'UserModule'!R1C1" tooltip="" display="UserModule"/>
+    <hyperlink ref="D16" location="'UserModuleMandatory'!R1C1" tooltip="" display="UserModuleMandatory"/>
   </hyperlinks>
+  <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -1628,97 +1862,97 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="30.5" style="6" customWidth="1"/>
-    <col min="2" max="2" width="27.8516" style="6" customWidth="1"/>
-    <col min="3" max="5" width="14.5" style="6" customWidth="1"/>
-    <col min="6" max="16384" width="14.5" style="6" customWidth="1"/>
+    <col min="1" max="1" width="30.5" style="25" customWidth="1"/>
+    <col min="2" max="2" width="27.8516" style="25" customWidth="1"/>
+    <col min="3" max="5" width="14.5" style="25" customWidth="1"/>
+    <col min="6" max="16384" width="14.5" style="25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.55" customHeight="1">
-      <c r="A1" t="s" s="7">
-        <v>6</v>
-      </c>
-      <c r="B1" t="s" s="7">
-        <v>7</v>
-      </c>
-      <c r="C1" t="s" s="8">
-        <v>8</v>
-      </c>
-      <c r="D1" t="s" s="8">
-        <v>9</v>
-      </c>
-      <c r="E1" s="9"/>
+      <c r="A1" t="s" s="26">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s" s="26">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s" s="27">
+        <v>14</v>
+      </c>
+      <c r="D1" t="s" s="27">
+        <v>15</v>
+      </c>
+      <c r="E1" s="28"/>
     </row>
     <row r="2" ht="17" customHeight="1">
-      <c r="A2" t="s" s="10">
-        <v>10</v>
-      </c>
-      <c r="B2" t="s" s="11">
-        <v>11</v>
-      </c>
-      <c r="C2" t="s" s="12">
-        <v>12</v>
-      </c>
-      <c r="D2" t="s" s="8">
-        <v>12</v>
-      </c>
-      <c r="E2" s="9"/>
+      <c r="A2" t="s" s="29">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s" s="30">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s" s="31">
+        <v>18</v>
+      </c>
+      <c r="D2" t="s" s="27">
+        <v>18</v>
+      </c>
+      <c r="E2" s="28"/>
     </row>
     <row r="3" ht="13.55" customHeight="1">
-      <c r="A3" s="13"/>
-      <c r="B3" s="13"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
+      <c r="A3" s="32"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
     </row>
     <row r="4" ht="13.55" customHeight="1">
-      <c r="A4" s="9"/>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
+      <c r="A4" s="28"/>
+      <c r="B4" s="28"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
     </row>
     <row r="5" ht="13.55" customHeight="1">
-      <c r="A5" s="9"/>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
+      <c r="A5" s="28"/>
+      <c r="B5" s="28"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="28"/>
     </row>
     <row r="6" ht="13.55" customHeight="1">
-      <c r="A6" s="9"/>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
+      <c r="A6" s="28"/>
+      <c r="B6" s="28"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
     </row>
     <row r="7" ht="13.55" customHeight="1">
-      <c r="A7" s="9"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
+      <c r="A7" s="28"/>
+      <c r="B7" s="28"/>
+      <c r="C7" s="28"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
     </row>
     <row r="8" ht="13.55" customHeight="1">
-      <c r="A8" s="9"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
+      <c r="A8" s="28"/>
+      <c r="B8" s="28"/>
+      <c r="C8" s="28"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="28"/>
     </row>
     <row r="9" ht="13.55" customHeight="1">
-      <c r="A9" s="9"/>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
+      <c r="A9" s="28"/>
+      <c r="B9" s="28"/>
+      <c r="C9" s="28"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="28"/>
     </row>
     <row r="10" ht="13.55" customHeight="1">
-      <c r="A10" s="9"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
+      <c r="A10" s="28"/>
+      <c r="B10" s="28"/>
+      <c r="C10" s="28"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="28"/>
     </row>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
@@ -1731,323 +1965,273 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:U10"/>
+  <dimension ref="A1:Q10"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="48.5" style="14" customWidth="1"/>
-    <col min="2" max="2" width="33.6719" style="14" customWidth="1"/>
-    <col min="3" max="21" width="8.67188" style="14" customWidth="1"/>
-    <col min="22" max="16384" width="14.5" style="14" customWidth="1"/>
+    <col min="1" max="1" width="48.5" style="33" customWidth="1"/>
+    <col min="2" max="2" width="33.6719" style="33" customWidth="1"/>
+    <col min="3" max="17" width="8.67188" style="33" customWidth="1"/>
+    <col min="18" max="16384" width="14.5" style="33" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.6" customHeight="1">
-      <c r="A1" t="s" s="15">
-        <v>14</v>
-      </c>
-      <c r="B1" t="s" s="15">
-        <v>15</v>
-      </c>
-      <c r="C1" t="s" s="15">
-        <v>16</v>
-      </c>
-      <c r="D1" t="s" s="15">
-        <v>17</v>
-      </c>
-      <c r="E1" t="s" s="15">
-        <v>18</v>
-      </c>
-      <c r="F1" t="s" s="15">
+      <c r="A1" t="s" s="34">
         <v>19</v>
       </c>
-      <c r="G1" t="s" s="15">
+      <c r="B1" t="s" s="34">
         <v>20</v>
       </c>
-      <c r="H1" t="s" s="15">
+      <c r="C1" t="s" s="34">
         <v>21</v>
       </c>
-      <c r="I1" t="s" s="15">
+      <c r="D1" t="s" s="34">
         <v>22</v>
       </c>
-      <c r="J1" t="s" s="15">
+      <c r="E1" t="s" s="34">
         <v>23</v>
       </c>
-      <c r="K1" t="s" s="15">
-        <v>7</v>
-      </c>
-      <c r="L1" t="s" s="15">
+      <c r="F1" t="s" s="34">
         <v>24</v>
       </c>
-      <c r="M1" t="s" s="15">
+      <c r="G1" t="s" s="34">
         <v>25</v>
       </c>
-      <c r="N1" t="s" s="15">
+      <c r="H1" t="s" s="34">
         <v>26</v>
       </c>
-      <c r="O1" t="s" s="15">
+      <c r="I1" t="s" s="34">
         <v>27</v>
       </c>
-      <c r="P1" t="s" s="15">
+      <c r="J1" t="s" s="34">
+        <v>13</v>
+      </c>
+      <c r="K1" t="s" s="34">
         <v>28</v>
       </c>
-      <c r="Q1" t="s" s="15">
+      <c r="L1" t="s" s="34">
         <v>29</v>
       </c>
-      <c r="R1" t="s" s="15">
+      <c r="M1" t="s" s="34">
         <v>30</v>
       </c>
-      <c r="S1" t="s" s="15">
+      <c r="N1" t="s" s="34">
         <v>31</v>
       </c>
-      <c r="T1" t="s" s="15">
+      <c r="O1" t="s" s="34">
         <v>32</v>
       </c>
-      <c r="U1" t="s" s="15">
+      <c r="P1" t="s" s="34">
         <v>33</v>
       </c>
+      <c r="Q1" t="s" s="34">
+        <v>34</v>
+      </c>
     </row>
     <row r="2" ht="19" customHeight="1">
-      <c r="A2" t="s" s="16">
-        <v>34</v>
-      </c>
-      <c r="B2" t="s" s="16">
+      <c r="A2" t="s" s="35">
         <v>35</v>
       </c>
-      <c r="C2" t="s" s="16">
+      <c r="B2" t="s" s="35">
         <v>36</v>
       </c>
-      <c r="D2" t="s" s="15">
+      <c r="C2" t="s" s="35">
         <v>37</v>
       </c>
-      <c r="E2" s="17"/>
-      <c r="F2" t="s" s="18">
+      <c r="D2" t="s" s="34">
         <v>38</v>
       </c>
-      <c r="G2" t="s" s="19">
+      <c r="E2" s="28"/>
+      <c r="F2" t="s" s="36">
         <v>39</v>
       </c>
-      <c r="H2" t="s" s="20">
+      <c r="G2" t="s" s="37">
         <v>40</v>
       </c>
-      <c r="I2" s="17"/>
-      <c r="J2" t="s" s="18">
+      <c r="H2" t="s" s="35">
         <v>41</v>
       </c>
-      <c r="K2" t="s" s="20">
+      <c r="I2" t="s" s="36">
         <v>42</v>
       </c>
-      <c r="L2" s="17"/>
-      <c r="M2" t="s" s="21">
-        <v>41</v>
-      </c>
-      <c r="N2" t="s" s="15">
+      <c r="J2" t="s" s="35">
         <v>43</v>
       </c>
-      <c r="O2" t="s" s="18">
+      <c r="K2" t="s" s="27">
         <v>44</v>
       </c>
-      <c r="P2" s="22">
-        <v>456768855</v>
-      </c>
-      <c r="Q2" s="17"/>
-      <c r="R2" t="s" s="21">
+      <c r="L2" t="s" s="38">
+        <v>42</v>
+      </c>
+      <c r="M2" t="s" s="36">
         <v>45</v>
       </c>
-      <c r="S2" t="s" s="21">
-        <v>41</v>
-      </c>
-      <c r="T2" t="s" s="21">
+      <c r="N2" t="s" s="38">
+        <v>44</v>
+      </c>
+      <c r="O2" t="s" s="38">
+        <v>42</v>
+      </c>
+      <c r="P2" t="s" s="38">
         <v>46</v>
       </c>
-      <c r="U2" t="s" s="21">
+      <c r="Q2" t="s" s="38">
         <v>47</v>
       </c>
     </row>
     <row r="3" ht="13.55" customHeight="1">
-      <c r="A3" s="9"/>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="9"/>
-      <c r="L3" s="9"/>
-      <c r="M3" s="9"/>
-      <c r="N3" s="9"/>
-      <c r="O3" s="9"/>
-      <c r="P3" s="9"/>
-      <c r="Q3" s="9"/>
-      <c r="R3" s="9"/>
-      <c r="S3" s="9"/>
-      <c r="T3" s="9"/>
-      <c r="U3" s="9"/>
+      <c r="A3" s="28"/>
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="28"/>
+      <c r="I3" s="28"/>
+      <c r="J3" s="28"/>
+      <c r="K3" s="28"/>
+      <c r="L3" s="28"/>
+      <c r="M3" s="28"/>
+      <c r="N3" s="28"/>
+      <c r="O3" s="28"/>
+      <c r="P3" s="28"/>
+      <c r="Q3" s="28"/>
     </row>
     <row r="4" ht="13.55" customHeight="1">
-      <c r="A4" s="9"/>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9"/>
-      <c r="K4" s="9"/>
-      <c r="L4" s="9"/>
-      <c r="M4" s="9"/>
-      <c r="N4" s="9"/>
-      <c r="O4" s="9"/>
-      <c r="P4" s="9"/>
-      <c r="Q4" s="9"/>
-      <c r="R4" s="9"/>
-      <c r="S4" s="9"/>
-      <c r="T4" s="9"/>
-      <c r="U4" s="9"/>
+      <c r="A4" s="28"/>
+      <c r="B4" s="28"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="28"/>
+      <c r="G4" s="28"/>
+      <c r="H4" s="28"/>
+      <c r="I4" s="28"/>
+      <c r="J4" s="28"/>
+      <c r="K4" s="28"/>
+      <c r="L4" s="28"/>
+      <c r="M4" s="28"/>
+      <c r="N4" s="28"/>
+      <c r="O4" s="28"/>
+      <c r="P4" s="28"/>
+      <c r="Q4" s="28"/>
     </row>
     <row r="5" ht="13.55" customHeight="1">
-      <c r="A5" s="9"/>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="9"/>
-      <c r="K5" s="9"/>
-      <c r="L5" s="9"/>
-      <c r="M5" s="9"/>
-      <c r="N5" s="9"/>
-      <c r="O5" s="9"/>
-      <c r="P5" s="9"/>
-      <c r="Q5" s="9"/>
-      <c r="R5" s="9"/>
-      <c r="S5" s="9"/>
-      <c r="T5" s="9"/>
-      <c r="U5" s="9"/>
+      <c r="A5" s="28"/>
+      <c r="B5" s="28"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="28"/>
+      <c r="G5" s="28"/>
+      <c r="H5" s="28"/>
+      <c r="I5" s="28"/>
+      <c r="J5" s="28"/>
+      <c r="K5" s="28"/>
+      <c r="L5" s="28"/>
+      <c r="M5" s="28"/>
+      <c r="N5" s="28"/>
+      <c r="O5" s="28"/>
+      <c r="P5" s="28"/>
+      <c r="Q5" s="28"/>
     </row>
     <row r="6" ht="13.55" customHeight="1">
-      <c r="A6" s="9"/>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9"/>
-      <c r="J6" s="9"/>
-      <c r="K6" s="9"/>
-      <c r="L6" s="9"/>
-      <c r="M6" s="9"/>
-      <c r="N6" s="9"/>
-      <c r="O6" s="9"/>
-      <c r="P6" s="9"/>
-      <c r="Q6" s="9"/>
-      <c r="R6" s="9"/>
-      <c r="S6" s="9"/>
-      <c r="T6" s="9"/>
-      <c r="U6" s="9"/>
+      <c r="A6" s="28"/>
+      <c r="B6" s="28"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="28"/>
+      <c r="G6" s="28"/>
+      <c r="H6" s="28"/>
+      <c r="I6" s="28"/>
+      <c r="J6" s="28"/>
+      <c r="K6" s="28"/>
+      <c r="L6" s="28"/>
+      <c r="M6" s="28"/>
+      <c r="N6" s="28"/>
+      <c r="O6" s="28"/>
+      <c r="P6" s="28"/>
+      <c r="Q6" s="28"/>
     </row>
     <row r="7" ht="13.55" customHeight="1">
-      <c r="A7" s="9"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="9"/>
-      <c r="J7" s="9"/>
-      <c r="K7" s="9"/>
-      <c r="L7" s="9"/>
-      <c r="M7" s="9"/>
-      <c r="N7" s="9"/>
-      <c r="O7" s="9"/>
-      <c r="P7" s="9"/>
-      <c r="Q7" s="9"/>
-      <c r="R7" s="9"/>
-      <c r="S7" s="9"/>
-      <c r="T7" s="9"/>
-      <c r="U7" s="9"/>
+      <c r="A7" s="28"/>
+      <c r="B7" s="28"/>
+      <c r="C7" s="28"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="28"/>
+      <c r="G7" s="28"/>
+      <c r="H7" s="28"/>
+      <c r="I7" s="28"/>
+      <c r="J7" s="28"/>
+      <c r="K7" s="28"/>
+      <c r="L7" s="28"/>
+      <c r="M7" s="28"/>
+      <c r="N7" s="28"/>
+      <c r="O7" s="28"/>
+      <c r="P7" s="28"/>
+      <c r="Q7" s="28"/>
     </row>
     <row r="8" ht="13.55" customHeight="1">
-      <c r="A8" s="9"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="9"/>
-      <c r="K8" s="9"/>
-      <c r="L8" s="9"/>
-      <c r="M8" s="9"/>
-      <c r="N8" s="9"/>
-      <c r="O8" s="9"/>
-      <c r="P8" s="9"/>
-      <c r="Q8" s="9"/>
-      <c r="R8" s="9"/>
-      <c r="S8" s="9"/>
-      <c r="T8" s="9"/>
-      <c r="U8" s="9"/>
+      <c r="A8" s="28"/>
+      <c r="B8" s="28"/>
+      <c r="C8" s="28"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="28"/>
+      <c r="I8" s="28"/>
+      <c r="J8" s="28"/>
+      <c r="K8" s="28"/>
+      <c r="L8" s="28"/>
+      <c r="M8" s="28"/>
+      <c r="N8" s="28"/>
+      <c r="O8" s="28"/>
+      <c r="P8" s="28"/>
+      <c r="Q8" s="28"/>
     </row>
     <row r="9" ht="13.55" customHeight="1">
-      <c r="A9" s="9"/>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="9"/>
-      <c r="K9" s="9"/>
-      <c r="L9" s="9"/>
-      <c r="M9" s="9"/>
-      <c r="N9" s="9"/>
-      <c r="O9" s="9"/>
-      <c r="P9" s="9"/>
-      <c r="Q9" s="9"/>
-      <c r="R9" s="9"/>
-      <c r="S9" s="9"/>
-      <c r="T9" s="9"/>
-      <c r="U9" s="9"/>
+      <c r="A9" s="28"/>
+      <c r="B9" s="28"/>
+      <c r="C9" s="28"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="28"/>
+      <c r="F9" s="28"/>
+      <c r="G9" s="28"/>
+      <c r="H9" s="28"/>
+      <c r="I9" s="28"/>
+      <c r="J9" s="28"/>
+      <c r="K9" s="28"/>
+      <c r="L9" s="28"/>
+      <c r="M9" s="28"/>
+      <c r="N9" s="28"/>
+      <c r="O9" s="28"/>
+      <c r="P9" s="28"/>
+      <c r="Q9" s="28"/>
     </row>
     <row r="10" ht="13.55" customHeight="1">
-      <c r="A10" s="9"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
-      <c r="K10" s="9"/>
-      <c r="L10" s="9"/>
-      <c r="M10" s="9"/>
-      <c r="N10" s="9"/>
-      <c r="O10" s="9"/>
-      <c r="P10" s="9"/>
-      <c r="Q10" s="9"/>
-      <c r="R10" s="9"/>
-      <c r="S10" s="9"/>
-      <c r="T10" s="9"/>
-      <c r="U10" s="9"/>
+      <c r="A10" s="28"/>
+      <c r="B10" s="28"/>
+      <c r="C10" s="28"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="28"/>
+      <c r="F10" s="28"/>
+      <c r="G10" s="28"/>
+      <c r="H10" s="28"/>
+      <c r="I10" s="28"/>
+      <c r="J10" s="28"/>
+      <c r="K10" s="28"/>
+      <c r="L10" s="28"/>
+      <c r="M10" s="28"/>
+      <c r="N10" s="28"/>
+      <c r="O10" s="28"/>
+      <c r="P10" s="28"/>
+      <c r="Q10" s="28"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2063,313 +2247,277 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:U10"/>
+  <dimension ref="A1:R10"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="48.5" style="23" customWidth="1"/>
-    <col min="2" max="2" width="33.6719" style="23" customWidth="1"/>
-    <col min="3" max="21" width="8.67188" style="23" customWidth="1"/>
-    <col min="22" max="16384" width="14.5" style="23" customWidth="1"/>
+    <col min="1" max="1" width="48.5" style="39" customWidth="1"/>
+    <col min="2" max="2" width="33.6719" style="39" customWidth="1"/>
+    <col min="3" max="18" width="8.67188" style="39" customWidth="1"/>
+    <col min="19" max="16384" width="14.5" style="39" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.6" customHeight="1">
-      <c r="A1" t="s" s="15">
-        <v>14</v>
-      </c>
-      <c r="B1" t="s" s="15">
-        <v>15</v>
-      </c>
-      <c r="C1" t="s" s="15">
-        <v>16</v>
-      </c>
-      <c r="D1" t="s" s="15">
-        <v>17</v>
-      </c>
-      <c r="E1" t="s" s="15">
-        <v>18</v>
-      </c>
-      <c r="F1" t="s" s="15">
+      <c r="A1" t="s" s="34">
         <v>19</v>
       </c>
-      <c r="G1" t="s" s="15">
+      <c r="B1" t="s" s="34">
         <v>20</v>
       </c>
-      <c r="H1" t="s" s="15">
+      <c r="C1" t="s" s="34">
         <v>21</v>
       </c>
-      <c r="I1" t="s" s="15">
+      <c r="D1" t="s" s="34">
         <v>22</v>
       </c>
-      <c r="J1" t="s" s="15">
+      <c r="E1" t="s" s="34">
         <v>23</v>
       </c>
-      <c r="K1" t="s" s="15">
-        <v>7</v>
-      </c>
-      <c r="L1" t="s" s="15">
+      <c r="F1" t="s" s="34">
         <v>24</v>
       </c>
-      <c r="M1" t="s" s="15">
+      <c r="G1" t="s" s="34">
         <v>25</v>
       </c>
-      <c r="N1" t="s" s="15">
+      <c r="H1" t="s" s="34">
         <v>26</v>
       </c>
-      <c r="O1" t="s" s="15">
+      <c r="I1" t="s" s="34">
+        <v>48</v>
+      </c>
+      <c r="J1" t="s" s="34">
         <v>27</v>
       </c>
-      <c r="P1" t="s" s="15">
+      <c r="K1" t="s" s="34">
+        <v>13</v>
+      </c>
+      <c r="L1" t="s" s="34">
         <v>28</v>
       </c>
-      <c r="Q1" t="s" s="15">
+      <c r="M1" t="s" s="34">
         <v>29</v>
       </c>
-      <c r="R1" t="s" s="15">
+      <c r="N1" t="s" s="34">
         <v>30</v>
       </c>
-      <c r="S1" t="s" s="15">
+      <c r="O1" t="s" s="34">
         <v>31</v>
       </c>
-      <c r="T1" t="s" s="15">
+      <c r="P1" t="s" s="34">
         <v>32</v>
       </c>
-      <c r="U1" t="s" s="15">
+      <c r="Q1" t="s" s="34">
         <v>33</v>
       </c>
+      <c r="R1" t="s" s="34">
+        <v>34</v>
+      </c>
     </row>
     <row r="2" ht="19" customHeight="1">
-      <c r="A2" t="s" s="8">
+      <c r="A2" t="s" s="27">
         <v>49</v>
       </c>
-      <c r="B2" t="s" s="8">
-        <v>35</v>
-      </c>
-      <c r="C2" t="s" s="8">
+      <c r="B2" t="s" s="27">
+        <v>36</v>
+      </c>
+      <c r="C2" t="s" s="27">
         <v>50</v>
       </c>
-      <c r="D2" t="s" s="15">
-        <v>37</v>
-      </c>
-      <c r="E2" s="9"/>
-      <c r="F2" t="s" s="8">
+      <c r="D2" t="s" s="34">
+        <v>38</v>
+      </c>
+      <c r="E2" s="28"/>
+      <c r="F2" t="s" s="27">
         <v>51</v>
       </c>
-      <c r="G2" t="s" s="19">
-        <v>39</v>
-      </c>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
-      <c r="J2" t="s" s="24">
-        <v>41</v>
-      </c>
-      <c r="K2" s="9"/>
-      <c r="L2" s="9"/>
-      <c r="M2" s="9"/>
-      <c r="N2" s="9"/>
-      <c r="O2" t="s" s="8">
+      <c r="G2" t="s" s="37">
+        <v>40</v>
+      </c>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
+      <c r="J2" t="s" s="36">
+        <v>42</v>
+      </c>
+      <c r="K2" s="28"/>
+      <c r="L2" s="28"/>
+      <c r="M2" s="28"/>
+      <c r="N2" t="s" s="27">
         <v>52</v>
       </c>
-      <c r="P2" s="9"/>
-      <c r="Q2" s="9"/>
-      <c r="R2" t="s" s="21">
-        <v>45</v>
-      </c>
-      <c r="S2" t="s" s="21">
-        <v>41</v>
-      </c>
-      <c r="T2" t="s" s="21">
+      <c r="O2" t="s" s="38">
+        <v>44</v>
+      </c>
+      <c r="P2" t="s" s="38">
+        <v>42</v>
+      </c>
+      <c r="Q2" t="s" s="38">
         <v>46</v>
       </c>
-      <c r="U2" t="s" s="21">
+      <c r="R2" t="s" s="38">
         <v>47</v>
       </c>
     </row>
     <row r="3" ht="13.55" customHeight="1">
-      <c r="A3" s="9"/>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="9"/>
-      <c r="L3" s="9"/>
-      <c r="M3" s="9"/>
-      <c r="N3" s="9"/>
-      <c r="O3" s="9"/>
-      <c r="P3" s="9"/>
-      <c r="Q3" s="9"/>
-      <c r="R3" s="9"/>
-      <c r="S3" s="9"/>
-      <c r="T3" s="9"/>
-      <c r="U3" s="9"/>
+      <c r="A3" s="28"/>
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="28"/>
+      <c r="I3" s="28"/>
+      <c r="J3" s="28"/>
+      <c r="K3" s="28"/>
+      <c r="L3" s="28"/>
+      <c r="M3" s="28"/>
+      <c r="N3" s="28"/>
+      <c r="O3" s="28"/>
+      <c r="P3" s="28"/>
+      <c r="Q3" s="28"/>
+      <c r="R3" s="28"/>
     </row>
     <row r="4" ht="13.55" customHeight="1">
-      <c r="A4" s="9"/>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9"/>
-      <c r="K4" s="9"/>
-      <c r="L4" s="9"/>
-      <c r="M4" s="9"/>
-      <c r="N4" s="9"/>
-      <c r="O4" s="9"/>
-      <c r="P4" s="9"/>
-      <c r="Q4" s="9"/>
-      <c r="R4" s="9"/>
-      <c r="S4" s="9"/>
-      <c r="T4" s="9"/>
-      <c r="U4" s="9"/>
+      <c r="A4" s="28"/>
+      <c r="B4" s="28"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="28"/>
+      <c r="G4" s="28"/>
+      <c r="H4" s="28"/>
+      <c r="I4" s="28"/>
+      <c r="J4" s="28"/>
+      <c r="K4" s="28"/>
+      <c r="L4" s="28"/>
+      <c r="M4" s="28"/>
+      <c r="N4" s="28"/>
+      <c r="O4" s="28"/>
+      <c r="P4" s="28"/>
+      <c r="Q4" s="28"/>
+      <c r="R4" s="28"/>
     </row>
     <row r="5" ht="13.55" customHeight="1">
-      <c r="A5" s="9"/>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="9"/>
-      <c r="K5" s="9"/>
-      <c r="L5" s="9"/>
-      <c r="M5" s="9"/>
-      <c r="N5" s="9"/>
-      <c r="O5" s="9"/>
-      <c r="P5" s="9"/>
-      <c r="Q5" s="9"/>
-      <c r="R5" s="9"/>
-      <c r="S5" s="9"/>
-      <c r="T5" s="9"/>
-      <c r="U5" s="9"/>
+      <c r="A5" s="28"/>
+      <c r="B5" s="28"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="28"/>
+      <c r="G5" s="28"/>
+      <c r="H5" s="28"/>
+      <c r="I5" s="28"/>
+      <c r="J5" s="28"/>
+      <c r="K5" s="28"/>
+      <c r="L5" s="28"/>
+      <c r="M5" s="28"/>
+      <c r="N5" s="28"/>
+      <c r="O5" s="28"/>
+      <c r="P5" s="28"/>
+      <c r="Q5" s="28"/>
+      <c r="R5" s="28"/>
     </row>
     <row r="6" ht="13.55" customHeight="1">
-      <c r="A6" s="9"/>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9"/>
-      <c r="J6" s="9"/>
-      <c r="K6" s="9"/>
-      <c r="L6" s="9"/>
-      <c r="M6" s="9"/>
-      <c r="N6" s="9"/>
-      <c r="O6" s="9"/>
-      <c r="P6" s="9"/>
-      <c r="Q6" s="9"/>
-      <c r="R6" s="9"/>
-      <c r="S6" s="9"/>
-      <c r="T6" s="9"/>
-      <c r="U6" s="9"/>
+      <c r="A6" s="28"/>
+      <c r="B6" s="28"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="28"/>
+      <c r="G6" s="28"/>
+      <c r="H6" s="28"/>
+      <c r="I6" s="28"/>
+      <c r="J6" s="28"/>
+      <c r="K6" s="28"/>
+      <c r="L6" s="28"/>
+      <c r="M6" s="28"/>
+      <c r="N6" s="28"/>
+      <c r="O6" s="28"/>
+      <c r="P6" s="28"/>
+      <c r="Q6" s="28"/>
+      <c r="R6" s="28"/>
     </row>
     <row r="7" ht="13.55" customHeight="1">
-      <c r="A7" s="9"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="9"/>
-      <c r="J7" s="9"/>
-      <c r="K7" s="9"/>
-      <c r="L7" s="9"/>
-      <c r="M7" s="9"/>
-      <c r="N7" s="9"/>
-      <c r="O7" s="9"/>
-      <c r="P7" s="9"/>
-      <c r="Q7" s="9"/>
-      <c r="R7" s="9"/>
-      <c r="S7" s="9"/>
-      <c r="T7" s="9"/>
-      <c r="U7" s="9"/>
+      <c r="A7" s="28"/>
+      <c r="B7" s="28"/>
+      <c r="C7" s="28"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="28"/>
+      <c r="G7" s="28"/>
+      <c r="H7" s="28"/>
+      <c r="I7" s="28"/>
+      <c r="J7" s="28"/>
+      <c r="K7" s="28"/>
+      <c r="L7" s="28"/>
+      <c r="M7" s="28"/>
+      <c r="N7" s="28"/>
+      <c r="O7" s="28"/>
+      <c r="P7" s="28"/>
+      <c r="Q7" s="28"/>
+      <c r="R7" s="28"/>
     </row>
     <row r="8" ht="13.55" customHeight="1">
-      <c r="A8" s="9"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="9"/>
-      <c r="K8" s="9"/>
-      <c r="L8" s="9"/>
-      <c r="M8" s="9"/>
-      <c r="N8" s="9"/>
-      <c r="O8" s="9"/>
-      <c r="P8" s="9"/>
-      <c r="Q8" s="9"/>
-      <c r="R8" s="9"/>
-      <c r="S8" s="9"/>
-      <c r="T8" s="9"/>
-      <c r="U8" s="9"/>
+      <c r="A8" s="28"/>
+      <c r="B8" s="28"/>
+      <c r="C8" s="28"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="28"/>
+      <c r="I8" s="28"/>
+      <c r="J8" s="28"/>
+      <c r="K8" s="28"/>
+      <c r="L8" s="28"/>
+      <c r="M8" s="28"/>
+      <c r="N8" s="28"/>
+      <c r="O8" s="28"/>
+      <c r="P8" s="28"/>
+      <c r="Q8" s="28"/>
+      <c r="R8" s="28"/>
     </row>
     <row r="9" ht="13.55" customHeight="1">
-      <c r="A9" s="9"/>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="9"/>
-      <c r="K9" s="9"/>
-      <c r="L9" s="9"/>
-      <c r="M9" s="9"/>
-      <c r="N9" s="9"/>
-      <c r="O9" s="9"/>
-      <c r="P9" s="9"/>
-      <c r="Q9" s="9"/>
-      <c r="R9" s="9"/>
-      <c r="S9" s="9"/>
-      <c r="T9" s="9"/>
-      <c r="U9" s="9"/>
+      <c r="A9" s="28"/>
+      <c r="B9" s="28"/>
+      <c r="C9" s="28"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="28"/>
+      <c r="F9" s="28"/>
+      <c r="G9" s="28"/>
+      <c r="H9" s="28"/>
+      <c r="I9" s="28"/>
+      <c r="J9" s="28"/>
+      <c r="K9" s="28"/>
+      <c r="L9" s="28"/>
+      <c r="M9" s="28"/>
+      <c r="N9" s="28"/>
+      <c r="O9" s="28"/>
+      <c r="P9" s="28"/>
+      <c r="Q9" s="28"/>
+      <c r="R9" s="28"/>
     </row>
     <row r="10" ht="13.55" customHeight="1">
-      <c r="A10" s="9"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
-      <c r="K10" s="9"/>
-      <c r="L10" s="9"/>
-      <c r="M10" s="9"/>
-      <c r="N10" s="9"/>
-      <c r="O10" s="9"/>
-      <c r="P10" s="9"/>
-      <c r="Q10" s="9"/>
-      <c r="R10" s="9"/>
-      <c r="S10" s="9"/>
-      <c r="T10" s="9"/>
-      <c r="U10" s="9"/>
+      <c r="A10" s="28"/>
+      <c r="B10" s="28"/>
+      <c r="C10" s="28"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="28"/>
+      <c r="F10" s="28"/>
+      <c r="G10" s="28"/>
+      <c r="H10" s="28"/>
+      <c r="I10" s="28"/>
+      <c r="J10" s="28"/>
+      <c r="K10" s="28"/>
+      <c r="L10" s="28"/>
+      <c r="M10" s="28"/>
+      <c r="N10" s="28"/>
+      <c r="O10" s="28"/>
+      <c r="P10" s="28"/>
+      <c r="Q10" s="28"/>
+      <c r="R10" s="28"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
schema validations and other batch validations
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Team_08_API Architects_LMSTestData.xlsx
+++ b/src/test/resources/TestData/Team_08_API Architects_LMSTestData.xlsx
@@ -3,7 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{AD128BFD-FE12-468B-A415-495FB9E253D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\priya\git\Team_08_APIArchitects_RestAssured\src\test\resources\TestData\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CDA6098-C6BA-4EEC-A379-7B19181D4AC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +20,6 @@
     <sheet name="PythonArray" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataChecksum="xiQ+14SZppxkpB3hF2CpN5YgPYHGoCsLamLy7CqNZLI="/>
@@ -25,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
   <si>
     <t>Username</t>
   </si>
@@ -109,6 +113,12 @@
   </si>
   <si>
     <t>null</t>
+  </si>
+  <si>
+    <t>updateBatchStatus</t>
+  </si>
+  <si>
+    <t>Inactive</t>
   </si>
 </sst>
 </file>
@@ -473,8 +483,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6792F2D-317A-4B56-B3C6-819C430D682E}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -506,7 +516,9 @@
       <c r="F1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="G1" s="4"/>
+      <c r="G1" s="4" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
@@ -526,6 +538,9 @@
       </c>
       <c r="F2" t="s">
         <v>27</v>
+      </c>
+      <c r="G2" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
All validation done.Create user Id done Positive and Negative scenerio.
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Team_08_API Architects_LMSTestData.xlsx
+++ b/src/test/resources/TestData/Team_08_API Architects_LMSTestData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="55">
   <si>
     <t>This document was exported from Numbers.  Each table was converted to an Excel worksheet. All other objects on each Numbers sheet were placed on separate worksheets. Please be aware that formula calculations may differ in Excel.</t>
   </si>
@@ -145,6 +145,9 @@
     <t>UserVisaStatus</t>
   </si>
   <si>
+    <t>InvalidValue</t>
+  </si>
+  <si>
     <t>CreatingRoleforAll</t>
   </si>
   <si>
@@ -190,6 +193,9 @@
   </si>
   <si>
     <t>H1B</t>
+  </si>
+  <si>
+    <t>Abc123@-*</t>
   </si>
   <si>
     <t>UserLogin</t>
@@ -1965,7 +1971,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:Q10"/>
+  <dimension ref="A1:X10"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1973,8 +1979,8 @@
   <cols>
     <col min="1" max="1" width="48.5" style="33" customWidth="1"/>
     <col min="2" max="2" width="33.6719" style="33" customWidth="1"/>
-    <col min="3" max="17" width="8.67188" style="33" customWidth="1"/>
-    <col min="18" max="16384" width="14.5" style="33" customWidth="1"/>
+    <col min="3" max="24" width="8.67188" style="33" customWidth="1"/>
+    <col min="25" max="16384" width="14.5" style="33" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.6" customHeight="1">
@@ -2029,57 +2035,75 @@
       <c r="Q1" t="s" s="34">
         <v>34</v>
       </c>
+      <c r="R1" t="s" s="34">
+        <v>35</v>
+      </c>
+      <c r="S1" s="34"/>
+      <c r="T1" s="34"/>
+      <c r="U1" s="34"/>
+      <c r="V1" s="34"/>
+      <c r="W1" s="34"/>
+      <c r="X1" s="34"/>
     </row>
     <row r="2" ht="19" customHeight="1">
       <c r="A2" t="s" s="35">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B2" t="s" s="35">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C2" t="s" s="35">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D2" t="s" s="34">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E2" s="28"/>
       <c r="F2" t="s" s="36">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G2" t="s" s="37">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H2" t="s" s="35">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="I2" t="s" s="36">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="J2" t="s" s="35">
+        <v>44</v>
+      </c>
+      <c r="K2" t="s" s="27">
+        <v>45</v>
+      </c>
+      <c r="L2" t="s" s="38">
         <v>43</v>
       </c>
-      <c r="K2" t="s" s="27">
-        <v>44</v>
-      </c>
-      <c r="L2" t="s" s="38">
-        <v>42</v>
-      </c>
       <c r="M2" t="s" s="36">
+        <v>46</v>
+      </c>
+      <c r="N2" t="s" s="38">
         <v>45</v>
       </c>
-      <c r="N2" t="s" s="38">
-        <v>44</v>
-      </c>
       <c r="O2" t="s" s="38">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="P2" t="s" s="38">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="Q2" t="s" s="38">
-        <v>47</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="R2" t="s" s="38">
+        <v>49</v>
+      </c>
+      <c r="S2" s="38"/>
+      <c r="T2" s="38"/>
+      <c r="U2" s="38"/>
+      <c r="V2" s="38"/>
+      <c r="W2" s="38"/>
+      <c r="X2" s="38"/>
     </row>
     <row r="3" ht="13.55" customHeight="1">
       <c r="A3" s="28"/>
@@ -2099,6 +2123,13 @@
       <c r="O3" s="28"/>
       <c r="P3" s="28"/>
       <c r="Q3" s="28"/>
+      <c r="R3" s="28"/>
+      <c r="S3" s="28"/>
+      <c r="T3" s="28"/>
+      <c r="U3" s="28"/>
+      <c r="V3" s="28"/>
+      <c r="W3" s="28"/>
+      <c r="X3" s="28"/>
     </row>
     <row r="4" ht="13.55" customHeight="1">
       <c r="A4" s="28"/>
@@ -2118,6 +2149,13 @@
       <c r="O4" s="28"/>
       <c r="P4" s="28"/>
       <c r="Q4" s="28"/>
+      <c r="R4" s="28"/>
+      <c r="S4" s="28"/>
+      <c r="T4" s="28"/>
+      <c r="U4" s="28"/>
+      <c r="V4" s="28"/>
+      <c r="W4" s="28"/>
+      <c r="X4" s="28"/>
     </row>
     <row r="5" ht="13.55" customHeight="1">
       <c r="A5" s="28"/>
@@ -2137,6 +2175,13 @@
       <c r="O5" s="28"/>
       <c r="P5" s="28"/>
       <c r="Q5" s="28"/>
+      <c r="R5" s="28"/>
+      <c r="S5" s="28"/>
+      <c r="T5" s="28"/>
+      <c r="U5" s="28"/>
+      <c r="V5" s="28"/>
+      <c r="W5" s="28"/>
+      <c r="X5" s="28"/>
     </row>
     <row r="6" ht="13.55" customHeight="1">
       <c r="A6" s="28"/>
@@ -2156,6 +2201,13 @@
       <c r="O6" s="28"/>
       <c r="P6" s="28"/>
       <c r="Q6" s="28"/>
+      <c r="R6" s="28"/>
+      <c r="S6" s="28"/>
+      <c r="T6" s="28"/>
+      <c r="U6" s="28"/>
+      <c r="V6" s="28"/>
+      <c r="W6" s="28"/>
+      <c r="X6" s="28"/>
     </row>
     <row r="7" ht="13.55" customHeight="1">
       <c r="A7" s="28"/>
@@ -2175,6 +2227,13 @@
       <c r="O7" s="28"/>
       <c r="P7" s="28"/>
       <c r="Q7" s="28"/>
+      <c r="R7" s="28"/>
+      <c r="S7" s="28"/>
+      <c r="T7" s="28"/>
+      <c r="U7" s="28"/>
+      <c r="V7" s="28"/>
+      <c r="W7" s="28"/>
+      <c r="X7" s="28"/>
     </row>
     <row r="8" ht="13.55" customHeight="1">
       <c r="A8" s="28"/>
@@ -2194,6 +2253,13 @@
       <c r="O8" s="28"/>
       <c r="P8" s="28"/>
       <c r="Q8" s="28"/>
+      <c r="R8" s="28"/>
+      <c r="S8" s="28"/>
+      <c r="T8" s="28"/>
+      <c r="U8" s="28"/>
+      <c r="V8" s="28"/>
+      <c r="W8" s="28"/>
+      <c r="X8" s="28"/>
     </row>
     <row r="9" ht="13.55" customHeight="1">
       <c r="A9" s="28"/>
@@ -2213,6 +2279,13 @@
       <c r="O9" s="28"/>
       <c r="P9" s="28"/>
       <c r="Q9" s="28"/>
+      <c r="R9" s="28"/>
+      <c r="S9" s="28"/>
+      <c r="T9" s="28"/>
+      <c r="U9" s="28"/>
+      <c r="V9" s="28"/>
+      <c r="W9" s="28"/>
+      <c r="X9" s="28"/>
     </row>
     <row r="10" ht="13.55" customHeight="1">
       <c r="A10" s="28"/>
@@ -2232,6 +2305,13 @@
       <c r="O10" s="28"/>
       <c r="P10" s="28"/>
       <c r="Q10" s="28"/>
+      <c r="R10" s="28"/>
+      <c r="S10" s="28"/>
+      <c r="T10" s="28"/>
+      <c r="U10" s="28"/>
+      <c r="V10" s="28"/>
+      <c r="W10" s="28"/>
+      <c r="X10" s="28"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2285,7 +2365,7 @@
         <v>26</v>
       </c>
       <c r="I1" t="s" s="34">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="J1" t="s" s="34">
         <v>27</v>
@@ -2317,46 +2397,46 @@
     </row>
     <row r="2" ht="19" customHeight="1">
       <c r="A2" t="s" s="27">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B2" t="s" s="27">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C2" t="s" s="27">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D2" t="s" s="34">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E2" s="28"/>
       <c r="F2" t="s" s="27">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="G2" t="s" s="37">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H2" s="28"/>
       <c r="I2" s="28"/>
       <c r="J2" t="s" s="36">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="K2" s="28"/>
       <c r="L2" s="28"/>
       <c r="M2" s="28"/>
       <c r="N2" t="s" s="27">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="O2" t="s" s="38">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="P2" t="s" s="38">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="Q2" t="s" s="38">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="R2" t="s" s="38">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" ht="13.55" customHeight="1">

</xml_diff>

<commit_message>
DONE WITH POST AND PUT
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Team_08_API Architects_LMSTestData.xlsx
+++ b/src/test/resources/TestData/Team_08_API Architects_LMSTestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\priya\git\Team_08_APIArchitects_RestAssured\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CDA6098-C6BA-4EEC-A379-7B19181D4AC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B13FCA92-3E75-479F-9390-6BFD6CAF8326}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
   <si>
     <t>Username</t>
   </si>
@@ -119,6 +119,12 @@
   </si>
   <si>
     <t>Inactive</t>
+  </si>
+  <si>
+    <t>updatebatchid</t>
+  </si>
+  <si>
+    <t>deletedbatchid</t>
   </si>
 </sst>
 </file>
@@ -481,10 +487,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6792F2D-317A-4B56-B3C6-819C430D682E}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -494,10 +500,13 @@
     <col min="3" max="3" width="14.7109375" customWidth="1"/>
     <col min="4" max="4" width="38.5703125" customWidth="1"/>
     <col min="5" max="5" width="30.7109375" customWidth="1"/>
-    <col min="6" max="6" width="35.5703125" customWidth="1"/>
+    <col min="6" max="6" width="51" customWidth="1"/>
+    <col min="7" max="7" width="19.7109375" customWidth="1"/>
+    <col min="8" max="8" width="15.42578125" customWidth="1"/>
+    <col min="9" max="9" width="36.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:9">
       <c r="A1" s="3" t="s">
         <v>21</v>
       </c>
@@ -519,8 +528,14 @@
       <c r="G1" s="4" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="H1" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -541,6 +556,12 @@
       </c>
       <c r="G2" t="s">
         <v>29</v>
+      </c>
+      <c r="H2">
+        <v>8545</v>
+      </c>
+      <c r="I2">
+        <v>8721</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Started Program Module from my End.
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Team_08_API Architects_LMSTestData.xlsx
+++ b/src/test/resources/TestData/Team_08_API Architects_LMSTestData.xlsx
@@ -9,12 +9,13 @@
     <sheet name="Login" sheetId="2" r:id="rId5"/>
     <sheet name="UserModule" sheetId="3" r:id="rId6"/>
     <sheet name="UserModuleMandatory" sheetId="4" r:id="rId7"/>
+    <sheet name="Program" sheetId="5" r:id="rId8"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="60">
   <si>
     <t>This document was exported from Numbers.  Each table was converted to an Excel worksheet. All other objects on each Numbers sheet were placed on separate worksheets. Please be aware that formula calculations may differ in Excel.</t>
   </si>
@@ -212,6 +213,21 @@
   <si>
     <t>TEAM</t>
   </si>
+  <si>
+    <t>Program</t>
+  </si>
+  <si>
+    <t>programDescription</t>
+  </si>
+  <si>
+    <t>programStatus</t>
+  </si>
+  <si>
+    <t>programId</t>
+  </si>
+  <si>
+    <t>Selenium Classes</t>
+  </si>
 </sst>
 </file>
 
@@ -220,7 +236,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -289,8 +305,19 @@
       <color indexed="8"/>
       <name val="Times Roman"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Helvetica"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -315,8 +342,20 @@
         <bgColor auto="1"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="18"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="14">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -465,13 +504,118 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="15"/>
+      </left>
+      <right style="thin">
+        <color indexed="15"/>
+      </right>
+      <top style="thin">
+        <color indexed="15"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="16"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="15"/>
+      </left>
+      <right style="thin">
+        <color indexed="16"/>
+      </right>
+      <top style="thin">
+        <color indexed="16"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="15"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="16"/>
+      </left>
+      <right style="thin">
+        <color indexed="15"/>
+      </right>
+      <top style="thin">
+        <color indexed="16"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="15"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="15"/>
+      </left>
+      <right style="thin">
+        <color indexed="15"/>
+      </right>
+      <top style="thin">
+        <color indexed="16"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="15"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="15"/>
+      </left>
+      <right style="thin">
+        <color indexed="16"/>
+      </right>
+      <top style="thin">
+        <color indexed="15"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="15"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="16"/>
+      </left>
+      <right style="thin">
+        <color indexed="15"/>
+      </right>
+      <top style="thin">
+        <color indexed="15"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="15"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="15"/>
+      </left>
+      <right style="thin">
+        <color indexed="15"/>
+      </right>
+      <top style="thin">
+        <color indexed="15"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="15"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -590,6 +734,39 @@
       <alignment vertical="bottom" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="17" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="18" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="19" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="20" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -615,6 +792,10 @@
       <rgbColor rgb="ffaaaaaa"/>
       <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ff0000ee"/>
+      <rgbColor rgb="ffa5a5a5"/>
+      <rgbColor rgb="ff3f3f3f"/>
+      <rgbColor rgb="ffbdc0bf"/>
+      <rgbColor rgb="ffdbdbdb"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -1835,6 +2016,22 @@
         <v>10</v>
       </c>
     </row>
+    <row r="17">
+      <c r="B17" t="s" s="3">
+        <v>55</v>
+      </c>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+    </row>
+    <row r="18">
+      <c r="B18" s="4"/>
+      <c r="C18" t="s" s="4">
+        <v>5</v>
+      </c>
+      <c r="D18" t="s" s="5">
+        <v>55</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B3:D3"/>
@@ -1848,6 +2045,7 @@
     <hyperlink ref="D12" location="'Login'!R1C1" tooltip="" display="Login"/>
     <hyperlink ref="D14" location="'UserModule'!R1C1" tooltip="" display="UserModule"/>
     <hyperlink ref="D16" location="'UserModuleMandatory'!R1C1" tooltip="" display="UserModuleMandatory"/>
+    <hyperlink ref="D18" location="'Program'!R1C1" tooltip="" display="Program"/>
   </hyperlinks>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
@@ -2609,4 +2807,112 @@
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
+      <pane topLeftCell="B2" xSplit="1" ySplit="1" activePane="bottomRight" state="frozen"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="15.4" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="5" width="16.3516" style="40" customWidth="1"/>
+    <col min="6" max="16384" width="16.3516" style="40" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="13.55" customHeight="1">
+      <c r="A1" t="s" s="41">
+        <v>56</v>
+      </c>
+      <c r="B1" t="s" s="42">
+        <v>57</v>
+      </c>
+      <c r="C1" t="s" s="42">
+        <v>58</v>
+      </c>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+    </row>
+    <row r="2" ht="13.1" customHeight="1">
+      <c r="A2" t="s" s="44">
+        <v>59</v>
+      </c>
+      <c r="B2" t="s" s="45">
+        <v>43</v>
+      </c>
+      <c r="C2" s="46">
+        <v>0</v>
+      </c>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+    </row>
+    <row r="3" ht="12.9" customHeight="1">
+      <c r="A3" s="48"/>
+      <c r="B3" s="49"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="50"/>
+    </row>
+    <row r="4" ht="12.9" customHeight="1">
+      <c r="A4" s="48"/>
+      <c r="B4" s="49"/>
+      <c r="C4" s="50"/>
+      <c r="D4" s="50"/>
+      <c r="E4" s="50"/>
+    </row>
+    <row r="5" ht="12.9" customHeight="1">
+      <c r="A5" s="48"/>
+      <c r="B5" s="49"/>
+      <c r="C5" s="50"/>
+      <c r="D5" s="50"/>
+      <c r="E5" s="50"/>
+    </row>
+    <row r="6" ht="12.9" customHeight="1">
+      <c r="A6" s="48"/>
+      <c r="B6" s="49"/>
+      <c r="C6" s="50"/>
+      <c r="D6" s="50"/>
+      <c r="E6" s="50"/>
+    </row>
+    <row r="7" ht="12.9" customHeight="1">
+      <c r="A7" s="48"/>
+      <c r="B7" s="49"/>
+      <c r="C7" s="50"/>
+      <c r="D7" s="50"/>
+      <c r="E7" s="50"/>
+    </row>
+    <row r="8" ht="12.9" customHeight="1">
+      <c r="A8" s="48"/>
+      <c r="B8" s="49"/>
+      <c r="C8" s="50"/>
+      <c r="D8" s="50"/>
+      <c r="E8" s="50"/>
+    </row>
+    <row r="9" ht="12.9" customHeight="1">
+      <c r="A9" s="48"/>
+      <c r="B9" s="49"/>
+      <c r="C9" s="50"/>
+      <c r="D9" s="50"/>
+      <c r="E9" s="50"/>
+    </row>
+    <row r="10" ht="12.9" customHeight="1">
+      <c r="A10" s="48"/>
+      <c r="B10" s="49"/>
+      <c r="C10" s="50"/>
+      <c r="D10" s="50"/>
+      <c r="E10" s="50"/>
+    </row>
+  </sheetData>
+  <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
changes done in GetProgramRequest,GetProgramModule
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Team_08_API Architects_LMSTestData.xlsx
+++ b/src/test/resources/TestData/Team_08_API Architects_LMSTestData.xlsx
@@ -1,13 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kswat\git\Team_08_APIArchitects_RestAssured\src\test\resources\TestData\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DCFE248-8393-4075-97F3-92F3FCEEA5D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="2475" yWindow="2025" windowWidth="15375" windowHeight="7785" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Login" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="PythonArray" sheetId="2" r:id="rId5"/>
+    <sheet name="Login" sheetId="1" r:id="rId1"/>
+    <sheet name="Program" sheetId="3" r:id="rId2"/>
+    <sheet name="Batch" sheetId="4" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="5" r:id="rId4"/>
+    <sheet name="PythonArray" sheetId="2" r:id="rId5"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataChecksum="xiQ+14SZppxkpB3hF2CpN5YgPYHGoCsLamLy7CqNZLI="/>
@@ -17,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
   <si>
     <t>Username</t>
   </si>
@@ -66,26 +78,67 @@
   <si>
     <t>search(input_list,num)</t>
   </si>
+  <si>
+    <t>programDescription</t>
+  </si>
+  <si>
+    <t>programStatus</t>
+  </si>
+  <si>
+    <t>Selenium Classes</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>BatchDescription</t>
+  </si>
+  <si>
+    <t>BatchNoOfClasses</t>
+  </si>
+  <si>
+    <t>BatchStatus</t>
+  </si>
+  <si>
+    <t>Sdet</t>
+  </si>
+  <si>
+    <t>InActive</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Menlo"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -93,7 +146,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -103,37 +156,42 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+  <cellXfs count="5">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -323,60 +381,162 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <cols>
+    <col min="1" max="1" width="30.5703125" customWidth="1"/>
+    <col min="2" max="2" width="27.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{287BA625-3A1E-4F32-910C-057B33D91932}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="22" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6792F2D-317A-4B56-B3C6-819C430D682E}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="17.42578125" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="3"/>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0973ABCC-0DFB-4CD7-A279-D6A93CDE91D4}">
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
-  <cols>
-    <col customWidth="1" min="1" max="1" width="30.57"/>
-    <col customWidth="1" min="2" max="2" width="27.86"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-  </sheetData>
-  <drawing r:id="rId1"/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="48.43"/>
-    <col customWidth="1" min="2" max="2" width="33.71"/>
-    <col customWidth="1" min="3" max="26" width="8.71"/>
+    <col min="1" max="1" width="48.42578125" customWidth="1"/>
+    <col min="2" max="2" width="33.7109375" customWidth="1"/>
+    <col min="3" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -384,7 +544,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -392,50 +552,48 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:2">
       <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:2">
       <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
     </row>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Coded Program Module from start , then integrated Login ProgramModule, UserModule-HAlf,UserProgramBatchMAp module.
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Team_08_API Architects_LMSTestData.xlsx
+++ b/src/test/resources/TestData/Team_08_API Architects_LMSTestData.xlsx
@@ -7,14 +7,15 @@
   <sheets>
     <sheet name="Export Summary" sheetId="1" r:id="rId4"/>
     <sheet name="Login" sheetId="2" r:id="rId5"/>
-    <sheet name="UserModule" sheetId="3" r:id="rId6"/>
-    <sheet name="UserModuleMandatory" sheetId="4" r:id="rId7"/>
+    <sheet name="Program" sheetId="3" r:id="rId6"/>
+    <sheet name="UserModule" sheetId="4" r:id="rId7"/>
+    <sheet name="UserModuleMandatory" sheetId="5" r:id="rId8"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="67">
   <si>
     <t>This document was exported from Numbers.  Each table was converted to an Excel worksheet. All other objects on each Numbers sheet were placed on separate worksheets. Please be aware that formula calculations may differ in Excel.</t>
   </si>
@@ -97,6 +98,45 @@
     <t>abc</t>
   </si>
   <si>
+    <t>Program</t>
+  </si>
+  <si>
+    <t>programDescription</t>
+  </si>
+  <si>
+    <t>programStatus</t>
+  </si>
+  <si>
+    <t>programId</t>
+  </si>
+  <si>
+    <t>updateProgramDescription</t>
+  </si>
+  <si>
+    <t>updateProgramStatus</t>
+  </si>
+  <si>
+    <t>InvalidProgramData</t>
+  </si>
+  <si>
+    <t>updateProgramDescription2</t>
+  </si>
+  <si>
+    <t>Selenium Classes</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>Java Classes</t>
+  </si>
+  <si>
+    <t>*12</t>
+  </si>
+  <si>
+    <t>API classes</t>
+  </si>
+  <si>
     <t>UserComments</t>
   </si>
   <si>
@@ -177,9 +217,6 @@
     <t>Georgia</t>
   </si>
   <si>
-    <t>Active</t>
-  </si>
-  <si>
     <t>Testuser</t>
   </si>
   <si>
@@ -220,7 +257,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="16">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -258,6 +295,22 @@
       <name val="Menlo Regular"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Helvetica"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color indexed="16"/>
+      <name val="Menlo Regular"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
       <sz val="12"/>
       <color indexed="8"/>
       <name val="Arial"/>
@@ -275,7 +328,7 @@
     <font>
       <u val="single"/>
       <sz val="12"/>
-      <color indexed="14"/>
+      <color indexed="18"/>
       <name val="Times Roman"/>
     </font>
     <font>
@@ -290,7 +343,7 @@
       <name val="Times Roman"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -315,8 +368,14 @@
         <bgColor auto="1"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="14">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -465,13 +524,118 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="14"/>
+      </left>
+      <right style="thin">
+        <color indexed="14"/>
+      </right>
+      <top style="thin">
+        <color indexed="14"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="15"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="14"/>
+      </left>
+      <right style="thin">
+        <color indexed="15"/>
+      </right>
+      <top style="thin">
+        <color indexed="15"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="14"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="15"/>
+      </left>
+      <right style="thin">
+        <color indexed="14"/>
+      </right>
+      <top style="thin">
+        <color indexed="15"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="14"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="14"/>
+      </left>
+      <right style="thin">
+        <color indexed="14"/>
+      </right>
+      <top style="thin">
+        <color indexed="15"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="14"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="14"/>
+      </left>
+      <right style="thin">
+        <color indexed="15"/>
+      </right>
+      <top style="thin">
+        <color indexed="14"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="14"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="15"/>
+      </left>
+      <right style="thin">
+        <color indexed="14"/>
+      </right>
+      <top style="thin">
+        <color indexed="14"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="14"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="14"/>
+      </left>
+      <right style="thin">
+        <color indexed="14"/>
+      </right>
+      <top style="thin">
+        <color indexed="14"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="14"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -574,19 +738,52 @@
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="4" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="4" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="4" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" readingOrder="1"/>
+    <xf numFmtId="49" fontId="7" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="18" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="19" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="20" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="10" fillId="4" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" readingOrder="1"/>
     </xf>
+    <xf numFmtId="49" fontId="11" fillId="4" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" readingOrder="1"/>
+    </xf>
     <xf numFmtId="49" fontId="12" fillId="4" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="4" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="4" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
@@ -614,6 +811,10 @@
       <rgbColor rgb="ff0000ff"/>
       <rgbColor rgb="ffaaaaaa"/>
       <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="ffa5a5a5"/>
+      <rgbColor rgb="ff3f3f3f"/>
+      <rgbColor rgb="ff3933ff"/>
+      <rgbColor rgb="ffdbdbdb"/>
       <rgbColor rgb="ff0000ee"/>
     </indexedColors>
   </colors>
@@ -1802,7 +2003,7 @@
     <row r="13" ht="13" customHeight="1">
       <c r="A13" s="10"/>
       <c r="B13" t="s" s="3">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
@@ -1815,13 +2016,13 @@
         <v>5</v>
       </c>
       <c r="D14" t="s" s="5">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="E14" s="24"/>
     </row>
     <row r="15">
       <c r="B15" t="s" s="3">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
@@ -1832,6 +2033,22 @@
         <v>5</v>
       </c>
       <c r="D16" t="s" s="5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="B17" t="s" s="3">
+        <v>10</v>
+      </c>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+    </row>
+    <row r="18">
+      <c r="B18" s="4"/>
+      <c r="C18" t="s" s="4">
+        <v>5</v>
+      </c>
+      <c r="D18" t="s" s="5">
         <v>10</v>
       </c>
     </row>
@@ -1846,8 +2063,9 @@
     <hyperlink ref="D12" location="'UserModule'!R1C1" tooltip="" display="UserModule"/>
     <hyperlink ref="D14" location="'UserModuleMandatory'!R1C1" tooltip="" display="UserModuleMandatory"/>
     <hyperlink ref="D12" location="'Login'!R1C1" tooltip="" display="Login"/>
-    <hyperlink ref="D14" location="'UserModule'!R1C1" tooltip="" display="UserModule"/>
-    <hyperlink ref="D16" location="'UserModuleMandatory'!R1C1" tooltip="" display="UserModuleMandatory"/>
+    <hyperlink ref="D14" location="'Program'!R1C1" tooltip="" display="Program"/>
+    <hyperlink ref="D16" location="'UserModule'!R1C1" tooltip="" display="UserModule"/>
+    <hyperlink ref="D18" location="'UserModuleMandatory'!R1C1" tooltip="" display="UserModuleMandatory"/>
   </hyperlinks>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
@@ -1971,139 +2189,283 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:G10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
+      <pane topLeftCell="B2" xSplit="1" ySplit="1" activePane="bottomRight" state="frozen"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="15.4" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="7" width="16.3516" style="33" customWidth="1"/>
+    <col min="8" max="16384" width="16.3516" style="33" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="14.55" customHeight="1">
+      <c r="A1" t="s" s="34">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s" s="35">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s" s="35">
+        <v>22</v>
+      </c>
+      <c r="D1" t="s" s="36">
+        <v>23</v>
+      </c>
+      <c r="E1" t="s" s="36">
+        <v>24</v>
+      </c>
+      <c r="F1" t="s" s="35">
+        <v>25</v>
+      </c>
+      <c r="G1" t="s" s="36">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" ht="13.1" customHeight="1">
+      <c r="A2" t="s" s="37">
+        <v>27</v>
+      </c>
+      <c r="B2" t="s" s="38">
+        <v>28</v>
+      </c>
+      <c r="C2" s="39">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s" s="40">
+        <v>29</v>
+      </c>
+      <c r="E2" t="s" s="40">
+        <v>28</v>
+      </c>
+      <c r="F2" t="s" s="40">
+        <v>30</v>
+      </c>
+      <c r="G2" t="s" s="40">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" ht="12.9" customHeight="1">
+      <c r="A3" s="41"/>
+      <c r="B3" s="42"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+    </row>
+    <row r="4" ht="12.9" customHeight="1">
+      <c r="A4" s="41"/>
+      <c r="B4" s="42"/>
+      <c r="C4" s="43"/>
+      <c r="D4" s="43"/>
+      <c r="E4" s="43"/>
+      <c r="F4" s="43"/>
+      <c r="G4" s="43"/>
+    </row>
+    <row r="5" ht="12.9" customHeight="1">
+      <c r="A5" s="41"/>
+      <c r="B5" s="42"/>
+      <c r="C5" s="43"/>
+      <c r="D5" s="43"/>
+      <c r="E5" s="43"/>
+      <c r="F5" s="43"/>
+      <c r="G5" s="43"/>
+    </row>
+    <row r="6" ht="12.9" customHeight="1">
+      <c r="A6" s="41"/>
+      <c r="B6" s="42"/>
+      <c r="C6" s="43"/>
+      <c r="D6" s="43"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="43"/>
+      <c r="G6" s="43"/>
+    </row>
+    <row r="7" ht="12.9" customHeight="1">
+      <c r="A7" s="41"/>
+      <c r="B7" s="42"/>
+      <c r="C7" s="43"/>
+      <c r="D7" s="43"/>
+      <c r="E7" s="43"/>
+      <c r="F7" s="43"/>
+      <c r="G7" s="43"/>
+    </row>
+    <row r="8" ht="12.9" customHeight="1">
+      <c r="A8" s="41"/>
+      <c r="B8" s="42"/>
+      <c r="C8" s="43"/>
+      <c r="D8" s="43"/>
+      <c r="E8" s="43"/>
+      <c r="F8" s="43"/>
+      <c r="G8" s="43"/>
+    </row>
+    <row r="9" ht="12.9" customHeight="1">
+      <c r="A9" s="41"/>
+      <c r="B9" s="42"/>
+      <c r="C9" s="43"/>
+      <c r="D9" s="43"/>
+      <c r="E9" s="43"/>
+      <c r="F9" s="43"/>
+      <c r="G9" s="43"/>
+    </row>
+    <row r="10" ht="12.9" customHeight="1">
+      <c r="A10" s="41"/>
+      <c r="B10" s="42"/>
+      <c r="C10" s="43"/>
+      <c r="D10" s="43"/>
+      <c r="E10" s="43"/>
+      <c r="F10" s="43"/>
+      <c r="G10" s="43"/>
+    </row>
+  </sheetData>
+  <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:X10"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="48.5" style="33" customWidth="1"/>
-    <col min="2" max="2" width="33.6719" style="33" customWidth="1"/>
-    <col min="3" max="24" width="8.67188" style="33" customWidth="1"/>
-    <col min="25" max="16384" width="14.5" style="33" customWidth="1"/>
+    <col min="1" max="1" width="48.5" style="44" customWidth="1"/>
+    <col min="2" max="2" width="33.6719" style="44" customWidth="1"/>
+    <col min="3" max="24" width="8.67188" style="44" customWidth="1"/>
+    <col min="25" max="16384" width="14.5" style="44" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.6" customHeight="1">
-      <c r="A1" t="s" s="34">
-        <v>19</v>
-      </c>
-      <c r="B1" t="s" s="34">
-        <v>20</v>
-      </c>
-      <c r="C1" t="s" s="34">
-        <v>21</v>
-      </c>
-      <c r="D1" t="s" s="34">
-        <v>22</v>
-      </c>
-      <c r="E1" t="s" s="34">
-        <v>23</v>
-      </c>
-      <c r="F1" t="s" s="34">
-        <v>24</v>
-      </c>
-      <c r="G1" t="s" s="34">
-        <v>25</v>
-      </c>
-      <c r="H1" t="s" s="34">
-        <v>26</v>
-      </c>
-      <c r="I1" t="s" s="34">
-        <v>27</v>
-      </c>
-      <c r="J1" t="s" s="34">
+      <c r="A1" t="s" s="45">
+        <v>32</v>
+      </c>
+      <c r="B1" t="s" s="45">
+        <v>33</v>
+      </c>
+      <c r="C1" t="s" s="45">
+        <v>34</v>
+      </c>
+      <c r="D1" t="s" s="45">
+        <v>35</v>
+      </c>
+      <c r="E1" t="s" s="45">
+        <v>36</v>
+      </c>
+      <c r="F1" t="s" s="45">
+        <v>37</v>
+      </c>
+      <c r="G1" t="s" s="45">
+        <v>38</v>
+      </c>
+      <c r="H1" t="s" s="45">
+        <v>39</v>
+      </c>
+      <c r="I1" t="s" s="45">
+        <v>40</v>
+      </c>
+      <c r="J1" t="s" s="45">
         <v>13</v>
       </c>
-      <c r="K1" t="s" s="34">
+      <c r="K1" t="s" s="45">
+        <v>41</v>
+      </c>
+      <c r="L1" t="s" s="45">
+        <v>42</v>
+      </c>
+      <c r="M1" t="s" s="45">
+        <v>43</v>
+      </c>
+      <c r="N1" t="s" s="45">
+        <v>44</v>
+      </c>
+      <c r="O1" t="s" s="45">
+        <v>45</v>
+      </c>
+      <c r="P1" t="s" s="45">
+        <v>46</v>
+      </c>
+      <c r="Q1" t="s" s="45">
+        <v>47</v>
+      </c>
+      <c r="R1" t="s" s="45">
+        <v>48</v>
+      </c>
+      <c r="S1" s="45"/>
+      <c r="T1" s="45"/>
+      <c r="U1" s="45"/>
+      <c r="V1" s="45"/>
+      <c r="W1" s="45"/>
+      <c r="X1" s="45"/>
+    </row>
+    <row r="2" ht="19" customHeight="1">
+      <c r="A2" t="s" s="46">
+        <v>49</v>
+      </c>
+      <c r="B2" t="s" s="46">
+        <v>50</v>
+      </c>
+      <c r="C2" t="s" s="46">
+        <v>51</v>
+      </c>
+      <c r="D2" t="s" s="45">
+        <v>52</v>
+      </c>
+      <c r="E2" s="28"/>
+      <c r="F2" t="s" s="47">
+        <v>53</v>
+      </c>
+      <c r="G2" t="s" s="48">
+        <v>54</v>
+      </c>
+      <c r="H2" t="s" s="46">
+        <v>55</v>
+      </c>
+      <c r="I2" t="s" s="47">
         <v>28</v>
       </c>
-      <c r="L1" t="s" s="34">
-        <v>29</v>
-      </c>
-      <c r="M1" t="s" s="34">
-        <v>30</v>
-      </c>
-      <c r="N1" t="s" s="34">
-        <v>31</v>
-      </c>
-      <c r="O1" t="s" s="34">
-        <v>32</v>
-      </c>
-      <c r="P1" t="s" s="34">
-        <v>33</v>
-      </c>
-      <c r="Q1" t="s" s="34">
-        <v>34</v>
-      </c>
-      <c r="R1" t="s" s="34">
-        <v>35</v>
-      </c>
-      <c r="S1" s="34"/>
-      <c r="T1" s="34"/>
-      <c r="U1" s="34"/>
-      <c r="V1" s="34"/>
-      <c r="W1" s="34"/>
-      <c r="X1" s="34"/>
-    </row>
-    <row r="2" ht="19" customHeight="1">
-      <c r="A2" t="s" s="35">
-        <v>36</v>
-      </c>
-      <c r="B2" t="s" s="35">
-        <v>37</v>
-      </c>
-      <c r="C2" t="s" s="35">
-        <v>38</v>
-      </c>
-      <c r="D2" t="s" s="34">
-        <v>39</v>
-      </c>
-      <c r="E2" s="28"/>
-      <c r="F2" t="s" s="36">
-        <v>40</v>
-      </c>
-      <c r="G2" t="s" s="37">
-        <v>41</v>
-      </c>
-      <c r="H2" t="s" s="35">
-        <v>42</v>
-      </c>
-      <c r="I2" t="s" s="36">
-        <v>43</v>
-      </c>
-      <c r="J2" t="s" s="35">
-        <v>44</v>
+      <c r="J2" t="s" s="46">
+        <v>56</v>
       </c>
       <c r="K2" t="s" s="27">
-        <v>45</v>
-      </c>
-      <c r="L2" t="s" s="38">
-        <v>43</v>
-      </c>
-      <c r="M2" t="s" s="36">
-        <v>46</v>
-      </c>
-      <c r="N2" t="s" s="38">
-        <v>45</v>
-      </c>
-      <c r="O2" t="s" s="38">
-        <v>43</v>
-      </c>
-      <c r="P2" t="s" s="38">
-        <v>47</v>
-      </c>
-      <c r="Q2" t="s" s="38">
-        <v>48</v>
-      </c>
-      <c r="R2" t="s" s="38">
-        <v>49</v>
-      </c>
-      <c r="S2" s="38"/>
-      <c r="T2" s="38"/>
-      <c r="U2" s="38"/>
-      <c r="V2" s="38"/>
-      <c r="W2" s="38"/>
-      <c r="X2" s="38"/>
+        <v>57</v>
+      </c>
+      <c r="L2" t="s" s="49">
+        <v>28</v>
+      </c>
+      <c r="M2" t="s" s="47">
+        <v>58</v>
+      </c>
+      <c r="N2" t="s" s="49">
+        <v>57</v>
+      </c>
+      <c r="O2" t="s" s="49">
+        <v>28</v>
+      </c>
+      <c r="P2" t="s" s="49">
+        <v>59</v>
+      </c>
+      <c r="Q2" t="s" s="49">
+        <v>60</v>
+      </c>
+      <c r="R2" t="s" s="49">
+        <v>61</v>
+      </c>
+      <c r="S2" s="49"/>
+      <c r="T2" s="49"/>
+      <c r="U2" s="49"/>
+      <c r="V2" s="49"/>
+      <c r="W2" s="49"/>
+      <c r="X2" s="49"/>
     </row>
     <row r="3" ht="13.55" customHeight="1">
       <c r="A3" s="28"/>
@@ -2325,7 +2687,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:R10"/>
   <sheetViews>
@@ -2333,110 +2695,110 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="48.5" style="39" customWidth="1"/>
-    <col min="2" max="2" width="33.6719" style="39" customWidth="1"/>
-    <col min="3" max="18" width="8.67188" style="39" customWidth="1"/>
-    <col min="19" max="16384" width="14.5" style="39" customWidth="1"/>
+    <col min="1" max="1" width="48.5" style="50" customWidth="1"/>
+    <col min="2" max="2" width="33.6719" style="50" customWidth="1"/>
+    <col min="3" max="18" width="8.67188" style="50" customWidth="1"/>
+    <col min="19" max="16384" width="14.5" style="50" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.6" customHeight="1">
-      <c r="A1" t="s" s="34">
-        <v>19</v>
-      </c>
-      <c r="B1" t="s" s="34">
-        <v>20</v>
-      </c>
-      <c r="C1" t="s" s="34">
-        <v>21</v>
-      </c>
-      <c r="D1" t="s" s="34">
-        <v>22</v>
-      </c>
-      <c r="E1" t="s" s="34">
-        <v>23</v>
-      </c>
-      <c r="F1" t="s" s="34">
-        <v>24</v>
-      </c>
-      <c r="G1" t="s" s="34">
-        <v>25</v>
-      </c>
-      <c r="H1" t="s" s="34">
-        <v>26</v>
-      </c>
-      <c r="I1" t="s" s="34">
-        <v>50</v>
-      </c>
-      <c r="J1" t="s" s="34">
-        <v>27</v>
-      </c>
-      <c r="K1" t="s" s="34">
+      <c r="A1" t="s" s="45">
+        <v>32</v>
+      </c>
+      <c r="B1" t="s" s="45">
+        <v>33</v>
+      </c>
+      <c r="C1" t="s" s="45">
+        <v>34</v>
+      </c>
+      <c r="D1" t="s" s="45">
+        <v>35</v>
+      </c>
+      <c r="E1" t="s" s="45">
+        <v>36</v>
+      </c>
+      <c r="F1" t="s" s="45">
+        <v>37</v>
+      </c>
+      <c r="G1" t="s" s="45">
+        <v>38</v>
+      </c>
+      <c r="H1" t="s" s="45">
+        <v>39</v>
+      </c>
+      <c r="I1" t="s" s="45">
+        <v>62</v>
+      </c>
+      <c r="J1" t="s" s="45">
+        <v>40</v>
+      </c>
+      <c r="K1" t="s" s="45">
         <v>13</v>
       </c>
-      <c r="L1" t="s" s="34">
-        <v>28</v>
-      </c>
-      <c r="M1" t="s" s="34">
-        <v>29</v>
-      </c>
-      <c r="N1" t="s" s="34">
-        <v>30</v>
-      </c>
-      <c r="O1" t="s" s="34">
-        <v>31</v>
-      </c>
-      <c r="P1" t="s" s="34">
-        <v>32</v>
-      </c>
-      <c r="Q1" t="s" s="34">
-        <v>33</v>
-      </c>
-      <c r="R1" t="s" s="34">
-        <v>34</v>
+      <c r="L1" t="s" s="45">
+        <v>41</v>
+      </c>
+      <c r="M1" t="s" s="45">
+        <v>42</v>
+      </c>
+      <c r="N1" t="s" s="45">
+        <v>43</v>
+      </c>
+      <c r="O1" t="s" s="45">
+        <v>44</v>
+      </c>
+      <c r="P1" t="s" s="45">
+        <v>45</v>
+      </c>
+      <c r="Q1" t="s" s="45">
+        <v>46</v>
+      </c>
+      <c r="R1" t="s" s="45">
+        <v>47</v>
       </c>
     </row>
     <row r="2" ht="19" customHeight="1">
       <c r="A2" t="s" s="27">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="B2" t="s" s="27">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="C2" t="s" s="27">
+        <v>64</v>
+      </c>
+      <c r="D2" t="s" s="45">
         <v>52</v>
-      </c>
-      <c r="D2" t="s" s="34">
-        <v>39</v>
       </c>
       <c r="E2" s="28"/>
       <c r="F2" t="s" s="27">
-        <v>53</v>
-      </c>
-      <c r="G2" t="s" s="37">
-        <v>41</v>
+        <v>65</v>
+      </c>
+      <c r="G2" t="s" s="48">
+        <v>54</v>
       </c>
       <c r="H2" s="28"/>
       <c r="I2" s="28"/>
-      <c r="J2" t="s" s="36">
-        <v>43</v>
+      <c r="J2" t="s" s="47">
+        <v>28</v>
       </c>
       <c r="K2" s="28"/>
       <c r="L2" s="28"/>
       <c r="M2" s="28"/>
       <c r="N2" t="s" s="27">
-        <v>54</v>
-      </c>
-      <c r="O2" t="s" s="38">
-        <v>45</v>
-      </c>
-      <c r="P2" t="s" s="38">
-        <v>43</v>
-      </c>
-      <c r="Q2" t="s" s="38">
-        <v>47</v>
-      </c>
-      <c r="R2" t="s" s="38">
-        <v>48</v>
+        <v>66</v>
+      </c>
+      <c r="O2" t="s" s="49">
+        <v>57</v>
+      </c>
+      <c r="P2" t="s" s="49">
+        <v>28</v>
+      </c>
+      <c r="Q2" t="s" s="49">
+        <v>59</v>
+      </c>
+      <c r="R2" t="s" s="49">
+        <v>60</v>
       </c>
     </row>
     <row r="3" ht="13.55" customHeight="1">

</xml_diff>

<commit_message>
doen with adding word "batch" at the end of wvery when and then
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Team_08_API Architects_LMSTestData.xlsx
+++ b/src/test/resources/TestData/Team_08_API Architects_LMSTestData.xlsx
@@ -3,12 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\priya\git\Team_08_APIArchitects_RestAssured\src\test\resources\TestData\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A2DDCB4-5149-4910-BC25-ABC40695FBD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{4E6C0BB5-C501-4D79-8A6A-F77277D5212D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,6 +15,7 @@
     <sheet name="PythonArray" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataChecksum="xiQ+14SZppxkpB3hF2CpN5YgPYHGoCsLamLy7CqNZLI="/>

</xml_diff>

<commit_message>
Except Batch Module everything is integrated
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Team_08_API Architects_LMSTestData.xlsx
+++ b/src/test/resources/TestData/Team_08_API Architects_LMSTestData.xlsx
@@ -8,14 +8,15 @@
     <sheet name="Export Summary" sheetId="1" r:id="rId4"/>
     <sheet name="Login" sheetId="2" r:id="rId5"/>
     <sheet name="Program" sheetId="3" r:id="rId6"/>
-    <sheet name="UserModule" sheetId="4" r:id="rId7"/>
-    <sheet name="UserModuleMandatory" sheetId="5" r:id="rId8"/>
+    <sheet name="Batch" sheetId="4" r:id="rId7"/>
+    <sheet name="UserModule" sheetId="5" r:id="rId8"/>
+    <sheet name="UserModuleMandatory" sheetId="6" r:id="rId9"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="89">
   <si>
     <t>This document was exported from Numbers.  Each table was converted to an Excel worksheet. All other objects on each Numbers sheet were placed on separate worksheets. Please be aware that formula calculations may differ in Excel.</t>
   </si>
@@ -137,6 +138,36 @@
     <t>API classes</t>
   </si>
   <si>
+    <t>Batch</t>
+  </si>
+  <si>
+    <t>BatchStatus</t>
+  </si>
+  <si>
+    <t>BatchNoOfClassesmissingadditonalfield</t>
+  </si>
+  <si>
+    <t>BatchStatusmissingadditonalfield</t>
+  </si>
+  <si>
+    <t>BatchDescriptionmissingadditionalfield</t>
+  </si>
+  <si>
+    <t>updateBatchStatus</t>
+  </si>
+  <si>
+    <t>updatebatchid</t>
+  </si>
+  <si>
+    <t>deletedbatchid</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t>Inactive</t>
+  </si>
+  <si>
     <t>UserComments</t>
   </si>
   <si>
@@ -186,6 +217,24 @@
   </si>
   <si>
     <t>InvalidValue</t>
+  </si>
+  <si>
+    <t>UpdateLastName</t>
+  </si>
+  <si>
+    <t>UpdateVisa</t>
+  </si>
+  <si>
+    <t>UpdateTimezone</t>
+  </si>
+  <si>
+    <t>UpdateFirstname</t>
+  </si>
+  <si>
+    <t>UpdateRoleStatus</t>
+  </si>
+  <si>
+    <t>UpdateRoleIds</t>
   </si>
   <si>
     <t>CreatingRoleforAll</t>
@@ -233,6 +282,24 @@
   </si>
   <si>
     <t>Abc123@-*</t>
+  </si>
+  <si>
+    <t>APITest</t>
+  </si>
+  <si>
+    <t>H4-EAD</t>
+  </si>
+  <si>
+    <t>CST</t>
+  </si>
+  <si>
+    <t>APIARCHITECTSTEAM</t>
+  </si>
+  <si>
+    <t>InActive</t>
+  </si>
+  <si>
+    <t>R02</t>
   </si>
   <si>
     <t>UserLogin</t>
@@ -635,7 +702,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -767,6 +834,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" borderId="20" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
@@ -2022,7 +2101,7 @@
     </row>
     <row r="15">
       <c r="B15" t="s" s="3">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
@@ -2033,12 +2112,12 @@
         <v>5</v>
       </c>
       <c r="D16" t="s" s="5">
-        <v>8</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17">
       <c r="B17" t="s" s="3">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
@@ -2049,6 +2128,22 @@
         <v>5</v>
       </c>
       <c r="D18" t="s" s="5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="B19" t="s" s="3">
+        <v>10</v>
+      </c>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+    </row>
+    <row r="20">
+      <c r="B20" s="4"/>
+      <c r="C20" t="s" s="4">
+        <v>5</v>
+      </c>
+      <c r="D20" t="s" s="5">
         <v>10</v>
       </c>
     </row>
@@ -2064,8 +2159,9 @@
     <hyperlink ref="D14" location="'UserModuleMandatory'!R1C1" tooltip="" display="UserModuleMandatory"/>
     <hyperlink ref="D12" location="'Login'!R1C1" tooltip="" display="Login"/>
     <hyperlink ref="D14" location="'Program'!R1C1" tooltip="" display="Program"/>
-    <hyperlink ref="D16" location="'UserModule'!R1C1" tooltip="" display="UserModule"/>
-    <hyperlink ref="D18" location="'UserModuleMandatory'!R1C1" tooltip="" display="UserModuleMandatory"/>
+    <hyperlink ref="D16" location="'Batch'!R2C1" tooltip="" display="Batch"/>
+    <hyperlink ref="D18" location="'UserModule'!R1C1" tooltip="" display="UserModule"/>
+    <hyperlink ref="D20" location="'UserModuleMandatory'!R1C1" tooltip="" display="UserModuleMandatory"/>
   </hyperlinks>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
@@ -2333,139 +2429,321 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A2:G11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
+      <pane topLeftCell="B3" xSplit="1" ySplit="2" activePane="bottomRight" state="frozen"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="15.4" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="7" width="16.3516" style="44" customWidth="1"/>
+    <col min="8" max="16384" width="16.3516" style="44" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="15.55" customHeight="1">
+      <c r="A1" t="s" s="45">
+        <v>5</v>
+      </c>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+    </row>
+    <row r="2" ht="13.55" customHeight="1">
+      <c r="A2" t="s" s="35">
+        <v>33</v>
+      </c>
+      <c r="B2" t="s" s="35">
+        <v>34</v>
+      </c>
+      <c r="C2" t="s" s="35">
+        <v>35</v>
+      </c>
+      <c r="D2" t="s" s="34">
+        <v>36</v>
+      </c>
+      <c r="E2" t="s" s="35">
+        <v>37</v>
+      </c>
+      <c r="F2" t="s" s="35">
+        <v>38</v>
+      </c>
+      <c r="G2" t="s" s="35">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" ht="11.1" customHeight="1">
+      <c r="A3" t="s" s="37">
+        <v>28</v>
+      </c>
+      <c r="B3" s="46">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s" s="47">
+        <v>28</v>
+      </c>
+      <c r="D3" t="s" s="47">
+        <v>40</v>
+      </c>
+      <c r="E3" t="s" s="47">
+        <v>41</v>
+      </c>
+      <c r="F3" s="39">
+        <v>8545</v>
+      </c>
+      <c r="G3" s="39">
+        <v>8721</v>
+      </c>
+    </row>
+    <row r="4" ht="12.9" customHeight="1">
+      <c r="A4" s="41"/>
+      <c r="B4" s="42"/>
+      <c r="C4" s="43"/>
+      <c r="D4" s="43"/>
+      <c r="E4" s="43"/>
+      <c r="F4" s="43"/>
+      <c r="G4" s="43"/>
+    </row>
+    <row r="5" ht="12.9" customHeight="1">
+      <c r="A5" s="41"/>
+      <c r="B5" s="42"/>
+      <c r="C5" s="43"/>
+      <c r="D5" s="43"/>
+      <c r="E5" s="43"/>
+      <c r="F5" s="43"/>
+      <c r="G5" s="43"/>
+    </row>
+    <row r="6" ht="12.9" customHeight="1">
+      <c r="A6" s="41"/>
+      <c r="B6" s="42"/>
+      <c r="C6" s="43"/>
+      <c r="D6" s="43"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="43"/>
+      <c r="G6" s="43"/>
+    </row>
+    <row r="7" ht="12.9" customHeight="1">
+      <c r="A7" s="41"/>
+      <c r="B7" s="42"/>
+      <c r="C7" s="43"/>
+      <c r="D7" s="43"/>
+      <c r="E7" s="43"/>
+      <c r="F7" s="43"/>
+      <c r="G7" s="43"/>
+    </row>
+    <row r="8" ht="12.9" customHeight="1">
+      <c r="A8" s="41"/>
+      <c r="B8" s="42"/>
+      <c r="C8" s="43"/>
+      <c r="D8" s="43"/>
+      <c r="E8" s="43"/>
+      <c r="F8" s="43"/>
+      <c r="G8" s="43"/>
+    </row>
+    <row r="9" ht="12.9" customHeight="1">
+      <c r="A9" s="41"/>
+      <c r="B9" s="42"/>
+      <c r="C9" s="43"/>
+      <c r="D9" s="43"/>
+      <c r="E9" s="43"/>
+      <c r="F9" s="43"/>
+      <c r="G9" s="43"/>
+    </row>
+    <row r="10" ht="12.9" customHeight="1">
+      <c r="A10" s="41"/>
+      <c r="B10" s="42"/>
+      <c r="C10" s="43"/>
+      <c r="D10" s="43"/>
+      <c r="E10" s="43"/>
+      <c r="F10" s="43"/>
+      <c r="G10" s="43"/>
+    </row>
+    <row r="11" ht="12.9" customHeight="1">
+      <c r="A11" s="41"/>
+      <c r="B11" s="42"/>
+      <c r="C11" s="43"/>
+      <c r="D11" s="43"/>
+      <c r="E11" s="43"/>
+      <c r="F11" s="43"/>
+      <c r="G11" s="43"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:G1"/>
+  </mergeCells>
+  <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:X10"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="48.5" style="44" customWidth="1"/>
-    <col min="2" max="2" width="33.6719" style="44" customWidth="1"/>
-    <col min="3" max="24" width="8.67188" style="44" customWidth="1"/>
-    <col min="25" max="16384" width="14.5" style="44" customWidth="1"/>
+    <col min="1" max="1" width="48.5" style="48" customWidth="1"/>
+    <col min="2" max="2" width="33.6719" style="48" customWidth="1"/>
+    <col min="3" max="24" width="8.67188" style="48" customWidth="1"/>
+    <col min="25" max="16384" width="14.5" style="48" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.6" customHeight="1">
-      <c r="A1" t="s" s="45">
-        <v>32</v>
-      </c>
-      <c r="B1" t="s" s="45">
-        <v>33</v>
-      </c>
-      <c r="C1" t="s" s="45">
-        <v>34</v>
-      </c>
-      <c r="D1" t="s" s="45">
-        <v>35</v>
-      </c>
-      <c r="E1" t="s" s="45">
-        <v>36</v>
-      </c>
-      <c r="F1" t="s" s="45">
-        <v>37</v>
-      </c>
-      <c r="G1" t="s" s="45">
-        <v>38</v>
-      </c>
-      <c r="H1" t="s" s="45">
-        <v>39</v>
-      </c>
-      <c r="I1" t="s" s="45">
-        <v>40</v>
-      </c>
-      <c r="J1" t="s" s="45">
+      <c r="A1" t="s" s="49">
+        <v>42</v>
+      </c>
+      <c r="B1" t="s" s="49">
+        <v>43</v>
+      </c>
+      <c r="C1" t="s" s="49">
+        <v>44</v>
+      </c>
+      <c r="D1" t="s" s="49">
+        <v>45</v>
+      </c>
+      <c r="E1" t="s" s="49">
+        <v>46</v>
+      </c>
+      <c r="F1" t="s" s="49">
+        <v>47</v>
+      </c>
+      <c r="G1" t="s" s="49">
+        <v>48</v>
+      </c>
+      <c r="H1" t="s" s="49">
+        <v>49</v>
+      </c>
+      <c r="I1" t="s" s="49">
+        <v>50</v>
+      </c>
+      <c r="J1" t="s" s="49">
         <v>13</v>
       </c>
-      <c r="K1" t="s" s="45">
-        <v>41</v>
-      </c>
-      <c r="L1" t="s" s="45">
-        <v>42</v>
-      </c>
-      <c r="M1" t="s" s="45">
-        <v>43</v>
-      </c>
-      <c r="N1" t="s" s="45">
-        <v>44</v>
-      </c>
-      <c r="O1" t="s" s="45">
-        <v>45</v>
-      </c>
-      <c r="P1" t="s" s="45">
-        <v>46</v>
-      </c>
-      <c r="Q1" t="s" s="45">
-        <v>47</v>
-      </c>
-      <c r="R1" t="s" s="45">
-        <v>48</v>
-      </c>
-      <c r="S1" s="45"/>
-      <c r="T1" s="45"/>
-      <c r="U1" s="45"/>
-      <c r="V1" s="45"/>
-      <c r="W1" s="45"/>
-      <c r="X1" s="45"/>
+      <c r="K1" t="s" s="49">
+        <v>51</v>
+      </c>
+      <c r="L1" t="s" s="49">
+        <v>52</v>
+      </c>
+      <c r="M1" t="s" s="49">
+        <v>53</v>
+      </c>
+      <c r="N1" t="s" s="49">
+        <v>54</v>
+      </c>
+      <c r="O1" t="s" s="49">
+        <v>55</v>
+      </c>
+      <c r="P1" t="s" s="49">
+        <v>56</v>
+      </c>
+      <c r="Q1" t="s" s="49">
+        <v>57</v>
+      </c>
+      <c r="R1" t="s" s="49">
+        <v>58</v>
+      </c>
+      <c r="S1" t="s" s="49">
+        <v>59</v>
+      </c>
+      <c r="T1" t="s" s="49">
+        <v>60</v>
+      </c>
+      <c r="U1" t="s" s="49">
+        <v>61</v>
+      </c>
+      <c r="V1" t="s" s="49">
+        <v>62</v>
+      </c>
+      <c r="W1" t="s" s="49">
+        <v>63</v>
+      </c>
+      <c r="X1" t="s" s="49">
+        <v>64</v>
+      </c>
     </row>
     <row r="2" ht="19" customHeight="1">
-      <c r="A2" t="s" s="46">
-        <v>49</v>
-      </c>
-      <c r="B2" t="s" s="46">
-        <v>50</v>
-      </c>
-      <c r="C2" t="s" s="46">
-        <v>51</v>
-      </c>
-      <c r="D2" t="s" s="45">
-        <v>52</v>
+      <c r="A2" t="s" s="50">
+        <v>65</v>
+      </c>
+      <c r="B2" t="s" s="50">
+        <v>66</v>
+      </c>
+      <c r="C2" t="s" s="50">
+        <v>67</v>
+      </c>
+      <c r="D2" t="s" s="49">
+        <v>68</v>
       </c>
       <c r="E2" s="28"/>
-      <c r="F2" t="s" s="47">
-        <v>53</v>
-      </c>
-      <c r="G2" t="s" s="48">
-        <v>54</v>
-      </c>
-      <c r="H2" t="s" s="46">
-        <v>55</v>
-      </c>
-      <c r="I2" t="s" s="47">
+      <c r="F2" t="s" s="51">
+        <v>69</v>
+      </c>
+      <c r="G2" t="s" s="52">
+        <v>70</v>
+      </c>
+      <c r="H2" t="s" s="50">
+        <v>71</v>
+      </c>
+      <c r="I2" t="s" s="51">
         <v>28</v>
       </c>
-      <c r="J2" t="s" s="46">
-        <v>56</v>
+      <c r="J2" t="s" s="50">
+        <v>72</v>
       </c>
       <c r="K2" t="s" s="27">
-        <v>57</v>
-      </c>
-      <c r="L2" t="s" s="49">
+        <v>73</v>
+      </c>
+      <c r="L2" t="s" s="53">
         <v>28</v>
       </c>
-      <c r="M2" t="s" s="47">
-        <v>58</v>
-      </c>
-      <c r="N2" t="s" s="49">
-        <v>57</v>
-      </c>
-      <c r="O2" t="s" s="49">
+      <c r="M2" t="s" s="51">
+        <v>74</v>
+      </c>
+      <c r="N2" t="s" s="53">
+        <v>73</v>
+      </c>
+      <c r="O2" t="s" s="53">
         <v>28</v>
       </c>
-      <c r="P2" t="s" s="49">
-        <v>59</v>
-      </c>
-      <c r="Q2" t="s" s="49">
-        <v>60</v>
-      </c>
-      <c r="R2" t="s" s="49">
-        <v>61</v>
-      </c>
-      <c r="S2" s="49"/>
-      <c r="T2" s="49"/>
-      <c r="U2" s="49"/>
-      <c r="V2" s="49"/>
-      <c r="W2" s="49"/>
-      <c r="X2" s="49"/>
+      <c r="P2" t="s" s="53">
+        <v>75</v>
+      </c>
+      <c r="Q2" t="s" s="53">
+        <v>76</v>
+      </c>
+      <c r="R2" t="s" s="53">
+        <v>77</v>
+      </c>
+      <c r="S2" t="s" s="53">
+        <v>78</v>
+      </c>
+      <c r="T2" t="s" s="53">
+        <v>79</v>
+      </c>
+      <c r="U2" t="s" s="53">
+        <v>80</v>
+      </c>
+      <c r="V2" t="s" s="53">
+        <v>81</v>
+      </c>
+      <c r="W2" t="s" s="53">
+        <v>82</v>
+      </c>
+      <c r="X2" t="s" s="27">
+        <v>83</v>
+      </c>
     </row>
     <row r="3" ht="13.55" customHeight="1">
       <c r="A3" s="28"/>
@@ -2687,7 +2965,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:R10"/>
   <sheetViews>
@@ -2695,110 +2973,110 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="48.5" style="50" customWidth="1"/>
-    <col min="2" max="2" width="33.6719" style="50" customWidth="1"/>
-    <col min="3" max="18" width="8.67188" style="50" customWidth="1"/>
-    <col min="19" max="16384" width="14.5" style="50" customWidth="1"/>
+    <col min="1" max="1" width="48.5" style="54" customWidth="1"/>
+    <col min="2" max="2" width="33.6719" style="54" customWidth="1"/>
+    <col min="3" max="18" width="8.67188" style="54" customWidth="1"/>
+    <col min="19" max="16384" width="14.5" style="54" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.6" customHeight="1">
-      <c r="A1" t="s" s="45">
-        <v>32</v>
-      </c>
-      <c r="B1" t="s" s="45">
-        <v>33</v>
-      </c>
-      <c r="C1" t="s" s="45">
-        <v>34</v>
-      </c>
-      <c r="D1" t="s" s="45">
-        <v>35</v>
-      </c>
-      <c r="E1" t="s" s="45">
-        <v>36</v>
-      </c>
-      <c r="F1" t="s" s="45">
-        <v>37</v>
-      </c>
-      <c r="G1" t="s" s="45">
-        <v>38</v>
-      </c>
-      <c r="H1" t="s" s="45">
-        <v>39</v>
-      </c>
-      <c r="I1" t="s" s="45">
-        <v>62</v>
-      </c>
-      <c r="J1" t="s" s="45">
-        <v>40</v>
-      </c>
-      <c r="K1" t="s" s="45">
+      <c r="A1" t="s" s="49">
+        <v>42</v>
+      </c>
+      <c r="B1" t="s" s="49">
+        <v>43</v>
+      </c>
+      <c r="C1" t="s" s="49">
+        <v>44</v>
+      </c>
+      <c r="D1" t="s" s="49">
+        <v>45</v>
+      </c>
+      <c r="E1" t="s" s="49">
+        <v>46</v>
+      </c>
+      <c r="F1" t="s" s="49">
+        <v>47</v>
+      </c>
+      <c r="G1" t="s" s="49">
+        <v>48</v>
+      </c>
+      <c r="H1" t="s" s="49">
+        <v>49</v>
+      </c>
+      <c r="I1" t="s" s="49">
+        <v>84</v>
+      </c>
+      <c r="J1" t="s" s="49">
+        <v>50</v>
+      </c>
+      <c r="K1" t="s" s="49">
         <v>13</v>
       </c>
-      <c r="L1" t="s" s="45">
-        <v>41</v>
-      </c>
-      <c r="M1" t="s" s="45">
-        <v>42</v>
-      </c>
-      <c r="N1" t="s" s="45">
-        <v>43</v>
-      </c>
-      <c r="O1" t="s" s="45">
-        <v>44</v>
-      </c>
-      <c r="P1" t="s" s="45">
-        <v>45</v>
-      </c>
-      <c r="Q1" t="s" s="45">
-        <v>46</v>
-      </c>
-      <c r="R1" t="s" s="45">
-        <v>47</v>
+      <c r="L1" t="s" s="49">
+        <v>51</v>
+      </c>
+      <c r="M1" t="s" s="49">
+        <v>52</v>
+      </c>
+      <c r="N1" t="s" s="49">
+        <v>53</v>
+      </c>
+      <c r="O1" t="s" s="49">
+        <v>54</v>
+      </c>
+      <c r="P1" t="s" s="49">
+        <v>55</v>
+      </c>
+      <c r="Q1" t="s" s="49">
+        <v>56</v>
+      </c>
+      <c r="R1" t="s" s="49">
+        <v>57</v>
       </c>
     </row>
     <row r="2" ht="19" customHeight="1">
       <c r="A2" t="s" s="27">
-        <v>63</v>
+        <v>85</v>
       </c>
       <c r="B2" t="s" s="27">
-        <v>50</v>
+        <v>66</v>
       </c>
       <c r="C2" t="s" s="27">
-        <v>64</v>
-      </c>
-      <c r="D2" t="s" s="45">
-        <v>52</v>
+        <v>86</v>
+      </c>
+      <c r="D2" t="s" s="49">
+        <v>68</v>
       </c>
       <c r="E2" s="28"/>
       <c r="F2" t="s" s="27">
-        <v>65</v>
-      </c>
-      <c r="G2" t="s" s="48">
-        <v>54</v>
+        <v>87</v>
+      </c>
+      <c r="G2" t="s" s="52">
+        <v>70</v>
       </c>
       <c r="H2" s="28"/>
       <c r="I2" s="28"/>
-      <c r="J2" t="s" s="47">
+      <c r="J2" t="s" s="51">
         <v>28</v>
       </c>
       <c r="K2" s="28"/>
       <c r="L2" s="28"/>
       <c r="M2" s="28"/>
       <c r="N2" t="s" s="27">
-        <v>66</v>
-      </c>
-      <c r="O2" t="s" s="49">
-        <v>57</v>
-      </c>
-      <c r="P2" t="s" s="49">
+        <v>88</v>
+      </c>
+      <c r="O2" t="s" s="53">
+        <v>73</v>
+      </c>
+      <c r="P2" t="s" s="53">
         <v>28</v>
       </c>
-      <c r="Q2" t="s" s="49">
-        <v>59</v>
-      </c>
-      <c r="R2" t="s" s="49">
-        <v>60</v>
+      <c r="Q2" t="s" s="53">
+        <v>75</v>
+      </c>
+      <c r="R2" t="s" s="53">
+        <v>76</v>
       </c>
     </row>
     <row r="3" ht="13.55" customHeight="1">

</xml_diff>

<commit_message>
Done All the Integration.. Running Well. Combined User Module and UserBatchProgramModule . Changed Test DAta.
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Team_08_API Architects_LMSTestData.xlsx
+++ b/src/test/resources/TestData/Team_08_API Architects_LMSTestData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="94">
   <si>
     <t>This document was exported from Numbers.  Each table was converted to an Excel worksheet. All other objects on each Numbers sheet were placed on separate worksheets. Please be aware that formula calculations may differ in Excel.</t>
   </si>
@@ -50,6 +50,34 @@
     </r>
   </si>
   <si>
+    <t>Program</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="12"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>Program</t>
+    </r>
+  </si>
+  <si>
+    <t>Batch</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="12"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>Batch</t>
+    </r>
+  </si>
+  <si>
     <t>UserModule</t>
   </si>
   <si>
@@ -99,9 +127,6 @@
     <t>abc</t>
   </si>
   <si>
-    <t>Program</t>
-  </si>
-  <si>
     <t>programDescription</t>
   </si>
   <si>
@@ -138,7 +163,10 @@
     <t>API classes</t>
   </si>
   <si>
-    <t>Batch</t>
+    <t>BatchDescription</t>
+  </si>
+  <si>
+    <t>BatchNoOfClasses</t>
   </si>
   <si>
     <t>BatchStatus</t>
@@ -160,6 +188,9 @@
   </si>
   <si>
     <t>deletedbatchid</t>
+  </si>
+  <si>
+    <t>4</t>
   </si>
   <si>
     <t>null</t>
@@ -431,7 +462,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="13"/>
+        <fgColor indexed="12"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
@@ -452,11 +483,11 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -465,7 +496,7 @@
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -473,17 +504,17 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </right>
       <top style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </left>
       <right/>
       <top/>
@@ -500,7 +531,7 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </right>
       <top/>
       <bottom/>
@@ -508,12 +539,23 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </left>
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="13"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
@@ -522,72 +564,61 @@
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="13"/>
+      </left>
+      <right style="thin">
+        <color indexed="13"/>
+      </right>
+      <top style="thin">
+        <color indexed="13"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="13"/>
+      </left>
+      <right style="thin">
+        <color indexed="13"/>
+      </right>
+      <top style="thin">
+        <color indexed="13"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </right>
-      <top/>
+      <top style="thin">
+        <color indexed="13"/>
+      </top>
       <bottom style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </left>
       <right style="thin">
-        <color indexed="12"/>
-      </right>
-      <top style="thin">
-        <color indexed="12"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="12"/>
-      </left>
-      <right style="thin">
-        <color indexed="12"/>
-      </right>
-      <top style="thin">
-        <color indexed="12"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="12"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="12"/>
-      </right>
-      <top style="thin">
-        <color indexed="12"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="12"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="12"/>
-      </left>
-      <right style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
@@ -724,28 +755,28 @@
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -763,20 +794,20 @@
     <xf numFmtId="49" fontId="4" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
@@ -805,47 +836,47 @@
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="7" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="8" fillId="4" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="18" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="19" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="20" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="5" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
@@ -888,8 +919,8 @@
       <rgbColor rgb="ff5e88b1"/>
       <rgbColor rgb="ffeef3f4"/>
       <rgbColor rgb="ff0000ff"/>
+      <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffaaaaaa"/>
-      <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffa5a5a5"/>
       <rgbColor rgb="ff3f3f3f"/>
       <rgbColor rgb="ff3933ff"/>
@@ -1959,7 +1990,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -2082,7 +2113,7 @@
     <row r="13" ht="13" customHeight="1">
       <c r="A13" s="10"/>
       <c r="B13" t="s" s="3">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
@@ -2095,57 +2126,69 @@
         <v>5</v>
       </c>
       <c r="D14" t="s" s="5">
-        <v>19</v>
-      </c>
-      <c r="E14" s="24"/>
-    </row>
-    <row r="15">
+        <v>8</v>
+      </c>
+      <c r="E14" s="21"/>
+    </row>
+    <row r="15" ht="13" customHeight="1">
+      <c r="A15" s="7"/>
       <c r="B15" t="s" s="3">
-        <v>32</v>
+        <v>10</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
-    </row>
-    <row r="16">
+      <c r="E15" s="9"/>
+    </row>
+    <row r="16" ht="13" customHeight="1">
+      <c r="A16" s="10"/>
       <c r="B16" s="4"/>
       <c r="C16" t="s" s="4">
         <v>5</v>
       </c>
       <c r="D16" t="s" s="5">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="17">
+        <v>10</v>
+      </c>
+      <c r="E16" s="12"/>
+    </row>
+    <row r="17" ht="13" customHeight="1">
+      <c r="A17" s="10"/>
       <c r="B17" t="s" s="3">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
-    </row>
-    <row r="18">
+      <c r="E17" s="12"/>
+    </row>
+    <row r="18" ht="13" customHeight="1">
+      <c r="A18" s="10"/>
       <c r="B18" s="4"/>
       <c r="C18" t="s" s="4">
         <v>5</v>
       </c>
       <c r="D18" t="s" s="5">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19">
+        <v>12</v>
+      </c>
+      <c r="E18" s="12"/>
+    </row>
+    <row r="19" ht="13" customHeight="1">
+      <c r="A19" s="10"/>
       <c r="B19" t="s" s="3">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
-    </row>
-    <row r="20">
+      <c r="E19" s="12"/>
+    </row>
+    <row r="20" ht="13" customHeight="1">
+      <c r="A20" s="20"/>
       <c r="B20" s="4"/>
       <c r="C20" t="s" s="4">
         <v>5</v>
       </c>
       <c r="D20" t="s" s="5">
-        <v>10</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="E20" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2155,11 +2198,14 @@
   <hyperlinks>
     <hyperlink ref="D10" location="'Export Summary'!R1C1" tooltip="" display="Export Summary"/>
     <hyperlink ref="D10" location="'Login'!R1C1" tooltip="" display="Login"/>
-    <hyperlink ref="D12" location="'UserModule'!R1C1" tooltip="" display="UserModule"/>
-    <hyperlink ref="D14" location="'UserModuleMandatory'!R1C1" tooltip="" display="UserModuleMandatory"/>
     <hyperlink ref="D12" location="'Login'!R1C1" tooltip="" display="Login"/>
     <hyperlink ref="D14" location="'Program'!R1C1" tooltip="" display="Program"/>
-    <hyperlink ref="D16" location="'Batch'!R2C1" tooltip="" display="Batch"/>
+    <hyperlink ref="D16" location="'(null)'!R1C1" tooltip="" display="Batch"/>
+    <hyperlink ref="D18" location="'UserModule'!R1C1" tooltip="" display="UserModule"/>
+    <hyperlink ref="D20" location="'UserModuleMandatory'!R1C1" tooltip="" display="UserModuleMandatory"/>
+    <hyperlink ref="D12" location="'Login'!R1C1" tooltip="" display="Login"/>
+    <hyperlink ref="D14" location="'Program'!R1C1" tooltip="" display="Program"/>
+    <hyperlink ref="D16" location="'Batch'!R1C1" tooltip="" display="Batch"/>
     <hyperlink ref="D18" location="'UserModule'!R1C1" tooltip="" display="UserModule"/>
     <hyperlink ref="D20" location="'UserModuleMandatory'!R1C1" tooltip="" display="UserModuleMandatory"/>
   </hyperlinks>
@@ -2190,31 +2236,31 @@
   <sheetData>
     <row r="1" ht="13.55" customHeight="1">
       <c r="A1" t="s" s="26">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B1" t="s" s="26">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C1" t="s" s="27">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="D1" t="s" s="27">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="E1" s="28"/>
     </row>
     <row r="2" ht="17" customHeight="1">
       <c r="A2" t="s" s="29">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B2" t="s" s="30">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C2" t="s" s="31">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="D2" t="s" s="27">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="E2" s="28"/>
     </row>
@@ -2290,9 +2336,7 @@
   </sheetPr>
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
-      <pane topLeftCell="B2" xSplit="1" ySplit="1" activePane="bottomRight" state="frozen"/>
-    </sheetView>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="15.4" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
@@ -2302,48 +2346,48 @@
   <sheetData>
     <row r="1" ht="14.55" customHeight="1">
       <c r="A1" t="s" s="34">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B1" t="s" s="35">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C1" t="s" s="35">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D1" t="s" s="36">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="E1" t="s" s="36">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F1" t="s" s="35">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="G1" t="s" s="36">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" ht="13.1" customHeight="1">
       <c r="A2" t="s" s="37">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B2" t="s" s="38">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C2" s="39">
         <v>0</v>
       </c>
       <c r="D2" t="s" s="40">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="E2" t="s" s="40">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="F2" t="s" s="40">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="G2" t="s" s="40">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" ht="12.9" customHeight="1">
@@ -2432,74 +2476,98 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:G11"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
-      <pane topLeftCell="B3" xSplit="1" ySplit="2" activePane="bottomRight" state="frozen"/>
-    </sheetView>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="15.4" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="7" width="16.3516" style="44" customWidth="1"/>
-    <col min="8" max="16384" width="16.3516" style="44" customWidth="1"/>
+    <col min="1" max="11" width="16.3516" style="44" customWidth="1"/>
+    <col min="12" max="16384" width="16.3516" style="44" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.55" customHeight="1">
-      <c r="A1" t="s" s="45">
-        <v>5</v>
-      </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-    </row>
-    <row r="2" ht="13.55" customHeight="1">
-      <c r="A2" t="s" s="35">
-        <v>33</v>
-      </c>
-      <c r="B2" t="s" s="35">
-        <v>34</v>
-      </c>
-      <c r="C2" t="s" s="35">
+    <row r="1" ht="14.55" customHeight="1">
+      <c r="A1" t="s" s="34">
         <v>35</v>
       </c>
-      <c r="D2" t="s" s="34">
+      <c r="B1" t="s" s="35">
         <v>36</v>
       </c>
-      <c r="E2" t="s" s="35">
+      <c r="C1" t="s" s="35">
         <v>37</v>
       </c>
-      <c r="F2" t="s" s="35">
+      <c r="D1" t="s" s="35">
         <v>38</v>
       </c>
-      <c r="G2" t="s" s="35">
+      <c r="E1" t="s" s="35">
         <v>39</v>
       </c>
-    </row>
-    <row r="3" ht="11.1" customHeight="1">
-      <c r="A3" t="s" s="37">
-        <v>28</v>
-      </c>
-      <c r="B3" s="46">
+      <c r="F1" t="s" s="34">
+        <v>40</v>
+      </c>
+      <c r="G1" t="s" s="35">
+        <v>41</v>
+      </c>
+      <c r="H1" t="s" s="35">
+        <v>42</v>
+      </c>
+      <c r="I1" t="s" s="35">
+        <v>43</v>
+      </c>
+      <c r="J1" t="s" s="34">
+        <v>35</v>
+      </c>
+      <c r="K1" t="s" s="35">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" ht="13.1" customHeight="1">
+      <c r="A2" t="s" s="37">
+        <v>30</v>
+      </c>
+      <c r="B2" s="45">
         <v>4</v>
       </c>
-      <c r="C3" t="s" s="47">
-        <v>28</v>
-      </c>
-      <c r="D3" t="s" s="47">
-        <v>40</v>
-      </c>
-      <c r="E3" t="s" s="47">
-        <v>41</v>
-      </c>
-      <c r="F3" s="39">
+      <c r="C2" t="s" s="46">
+        <v>31</v>
+      </c>
+      <c r="D2" t="s" s="46">
+        <v>44</v>
+      </c>
+      <c r="E2" t="s" s="46">
+        <v>31</v>
+      </c>
+      <c r="F2" t="s" s="47">
+        <v>45</v>
+      </c>
+      <c r="G2" t="s" s="47">
+        <v>46</v>
+      </c>
+      <c r="H2" s="39">
         <v>8545</v>
       </c>
-      <c r="G3" s="39">
+      <c r="I2" s="39">
         <v>8721</v>
       </c>
+      <c r="J2" t="s" s="37">
+        <v>30</v>
+      </c>
+      <c r="K2" s="45">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" ht="12.9" customHeight="1">
+      <c r="A3" s="41"/>
+      <c r="B3" s="42"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="43"/>
+      <c r="J3" s="43"/>
+      <c r="K3" s="43"/>
     </row>
     <row r="4" ht="12.9" customHeight="1">
       <c r="A4" s="41"/>
@@ -2509,6 +2577,10 @@
       <c r="E4" s="43"/>
       <c r="F4" s="43"/>
       <c r="G4" s="43"/>
+      <c r="H4" s="43"/>
+      <c r="I4" s="43"/>
+      <c r="J4" s="43"/>
+      <c r="K4" s="43"/>
     </row>
     <row r="5" ht="12.9" customHeight="1">
       <c r="A5" s="41"/>
@@ -2518,6 +2590,10 @@
       <c r="E5" s="43"/>
       <c r="F5" s="43"/>
       <c r="G5" s="43"/>
+      <c r="H5" s="43"/>
+      <c r="I5" s="43"/>
+      <c r="J5" s="43"/>
+      <c r="K5" s="43"/>
     </row>
     <row r="6" ht="12.9" customHeight="1">
       <c r="A6" s="41"/>
@@ -2527,6 +2603,10 @@
       <c r="E6" s="43"/>
       <c r="F6" s="43"/>
       <c r="G6" s="43"/>
+      <c r="H6" s="43"/>
+      <c r="I6" s="43"/>
+      <c r="J6" s="43"/>
+      <c r="K6" s="43"/>
     </row>
     <row r="7" ht="12.9" customHeight="1">
       <c r="A7" s="41"/>
@@ -2536,6 +2616,10 @@
       <c r="E7" s="43"/>
       <c r="F7" s="43"/>
       <c r="G7" s="43"/>
+      <c r="H7" s="43"/>
+      <c r="I7" s="43"/>
+      <c r="J7" s="43"/>
+      <c r="K7" s="43"/>
     </row>
     <row r="8" ht="12.9" customHeight="1">
       <c r="A8" s="41"/>
@@ -2545,6 +2629,10 @@
       <c r="E8" s="43"/>
       <c r="F8" s="43"/>
       <c r="G8" s="43"/>
+      <c r="H8" s="43"/>
+      <c r="I8" s="43"/>
+      <c r="J8" s="43"/>
+      <c r="K8" s="43"/>
     </row>
     <row r="9" ht="12.9" customHeight="1">
       <c r="A9" s="41"/>
@@ -2554,6 +2642,10 @@
       <c r="E9" s="43"/>
       <c r="F9" s="43"/>
       <c r="G9" s="43"/>
+      <c r="H9" s="43"/>
+      <c r="I9" s="43"/>
+      <c r="J9" s="43"/>
+      <c r="K9" s="43"/>
     </row>
     <row r="10" ht="12.9" customHeight="1">
       <c r="A10" s="41"/>
@@ -2563,20 +2655,12 @@
       <c r="E10" s="43"/>
       <c r="F10" s="43"/>
       <c r="G10" s="43"/>
-    </row>
-    <row r="11" ht="12.9" customHeight="1">
-      <c r="A11" s="41"/>
-      <c r="B11" s="42"/>
-      <c r="C11" s="43"/>
-      <c r="D11" s="43"/>
-      <c r="E11" s="43"/>
-      <c r="F11" s="43"/>
-      <c r="G11" s="43"/>
+      <c r="H10" s="43"/>
+      <c r="I10" s="43"/>
+      <c r="J10" s="43"/>
+      <c r="K10" s="43"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:G1"/>
-  </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
@@ -2601,148 +2685,148 @@
   <sheetData>
     <row r="1" ht="14.6" customHeight="1">
       <c r="A1" t="s" s="49">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="B1" t="s" s="49">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C1" t="s" s="49">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="D1" t="s" s="49">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="E1" t="s" s="49">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="F1" t="s" s="49">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="G1" t="s" s="49">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="H1" t="s" s="49">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="I1" t="s" s="49">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="J1" t="s" s="49">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="K1" t="s" s="49">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="L1" t="s" s="49">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="M1" t="s" s="49">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="N1" t="s" s="49">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="O1" t="s" s="49">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="P1" t="s" s="49">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="Q1" t="s" s="49">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="R1" t="s" s="49">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="S1" t="s" s="49">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="T1" t="s" s="49">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="U1" t="s" s="49">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="V1" t="s" s="49">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="W1" t="s" s="49">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="X1" t="s" s="49">
-        <v>64</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" ht="19" customHeight="1">
       <c r="A2" t="s" s="50">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="B2" t="s" s="50">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="C2" t="s" s="50">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="D2" t="s" s="49">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="E2" s="28"/>
       <c r="F2" t="s" s="51">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="G2" t="s" s="52">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="H2" t="s" s="50">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="I2" t="s" s="51">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="J2" t="s" s="50">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="K2" t="s" s="27">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="L2" t="s" s="53">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="M2" t="s" s="51">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="N2" t="s" s="53">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="O2" t="s" s="53">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="P2" t="s" s="53">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="Q2" t="s" s="53">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="R2" t="s" s="53">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="S2" t="s" s="53">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="T2" t="s" s="53">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="U2" t="s" s="53">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="V2" t="s" s="53">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="W2" t="s" s="53">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="X2" t="s" s="27">
-        <v>83</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" ht="13.55" customHeight="1">
@@ -2981,102 +3065,102 @@
   <sheetData>
     <row r="1" ht="14.6" customHeight="1">
       <c r="A1" t="s" s="49">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="B1" t="s" s="49">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C1" t="s" s="49">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="D1" t="s" s="49">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="E1" t="s" s="49">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="F1" t="s" s="49">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="G1" t="s" s="49">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="H1" t="s" s="49">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="I1" t="s" s="49">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="J1" t="s" s="49">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="K1" t="s" s="49">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="L1" t="s" s="49">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="M1" t="s" s="49">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="N1" t="s" s="49">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="O1" t="s" s="49">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="P1" t="s" s="49">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="Q1" t="s" s="49">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="R1" t="s" s="49">
-        <v>57</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" ht="19" customHeight="1">
       <c r="A2" t="s" s="27">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="B2" t="s" s="27">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="C2" t="s" s="27">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="D2" t="s" s="49">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="E2" s="28"/>
       <c r="F2" t="s" s="27">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="G2" t="s" s="52">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="H2" s="28"/>
       <c r="I2" s="28"/>
       <c r="J2" t="s" s="51">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="K2" s="28"/>
       <c r="L2" s="28"/>
       <c r="M2" s="28"/>
       <c r="N2" t="s" s="27">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="O2" t="s" s="53">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="P2" t="s" s="53">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="Q2" t="s" s="53">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="R2" t="s" s="53">
-        <v>76</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" ht="13.55" customHeight="1">

</xml_diff>